<commit_message>
Update Project Spyn Gantt Chart.xlsx
</commit_message>
<xml_diff>
--- a/Project Spyn Gantt Chart.xlsx
+++ b/Project Spyn Gantt Chart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tydng\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tydng\Desktop\FSE-100-Team-4-Sheibanian\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{569208D4-19E1-490E-9E73-6FBDF2E18445}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49679D53-7A36-4A85-B6EF-7613B86E3018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5820" yWindow="3165" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project schedule" sheetId="11" r:id="rId1"/>
@@ -1136,22 +1136,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="19" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="19" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="19" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1163,14 +1160,17 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="19" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="19" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="19" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -1654,10 +1654,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1866,8 +1862,8 @@
   </sheetPr>
   <dimension ref="A1:BL36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="F24" zoomScale="115" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="AU31" sqref="AU31"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="B1" zoomScale="115" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1893,29 +1889,29 @@
       <c r="E1" s="20"/>
       <c r="F1" s="21"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="115" t="s">
+      <c r="I1" s="114" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="116"/>
-      <c r="K1" s="116"/>
-      <c r="L1" s="116"/>
-      <c r="M1" s="116"/>
-      <c r="N1" s="116"/>
-      <c r="O1" s="116"/>
+      <c r="J1" s="115"/>
+      <c r="K1" s="115"/>
+      <c r="L1" s="115"/>
+      <c r="M1" s="115"/>
+      <c r="N1" s="115"/>
+      <c r="O1" s="115"/>
       <c r="P1" s="24"/>
-      <c r="Q1" s="114">
+      <c r="Q1" s="113">
         <f ca="1">TODAY()</f>
-        <v>45195</v>
-      </c>
-      <c r="R1" s="113"/>
-      <c r="S1" s="113"/>
-      <c r="T1" s="113"/>
-      <c r="U1" s="113"/>
-      <c r="V1" s="113"/>
-      <c r="W1" s="113"/>
-      <c r="X1" s="113"/>
-      <c r="Y1" s="113"/>
-      <c r="Z1" s="113"/>
+        <v>45204</v>
+      </c>
+      <c r="R1" s="112"/>
+      <c r="S1" s="112"/>
+      <c r="T1" s="112"/>
+      <c r="U1" s="112"/>
+      <c r="V1" s="112"/>
+      <c r="W1" s="112"/>
+      <c r="X1" s="112"/>
+      <c r="Y1" s="112"/>
+      <c r="Z1" s="112"/>
     </row>
     <row r="2" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B2" s="96" t="s">
@@ -1927,28 +1923,28 @@
       <c r="D2" s="22"/>
       <c r="E2" s="23"/>
       <c r="F2" s="22"/>
-      <c r="I2" s="115" t="s">
+      <c r="I2" s="114" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="116"/>
-      <c r="K2" s="116"/>
-      <c r="L2" s="116"/>
-      <c r="M2" s="116"/>
-      <c r="N2" s="116"/>
-      <c r="O2" s="116"/>
+      <c r="J2" s="115"/>
+      <c r="K2" s="115"/>
+      <c r="L2" s="115"/>
+      <c r="M2" s="115"/>
+      <c r="N2" s="115"/>
+      <c r="O2" s="115"/>
       <c r="P2" s="24"/>
-      <c r="Q2" s="112">
+      <c r="Q2" s="111">
         <v>1</v>
       </c>
-      <c r="R2" s="113"/>
-      <c r="S2" s="113"/>
-      <c r="T2" s="113"/>
-      <c r="U2" s="113"/>
-      <c r="V2" s="113"/>
-      <c r="W2" s="113"/>
-      <c r="X2" s="113"/>
-      <c r="Y2" s="113"/>
-      <c r="Z2" s="113"/>
+      <c r="R2" s="112"/>
+      <c r="S2" s="112"/>
+      <c r="T2" s="112"/>
+      <c r="U2" s="112"/>
+      <c r="V2" s="112"/>
+      <c r="W2" s="112"/>
+      <c r="X2" s="112"/>
+      <c r="Y2" s="112"/>
+      <c r="Z2" s="112"/>
     </row>
     <row r="3" spans="1:64" s="26" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13"/>
@@ -1957,78 +1953,78 @@
       </c>
       <c r="D3" s="27"/>
       <c r="E3" s="28"/>
-      <c r="I3" s="117" t="s">
+      <c r="I3" s="106" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="118"/>
-      <c r="K3" s="118"/>
-      <c r="L3" s="118"/>
-      <c r="M3" s="118"/>
-      <c r="N3" s="118"/>
-      <c r="O3" s="118"/>
-      <c r="P3" s="117" t="s">
+      <c r="J3" s="107"/>
+      <c r="K3" s="107"/>
+      <c r="L3" s="107"/>
+      <c r="M3" s="107"/>
+      <c r="N3" s="107"/>
+      <c r="O3" s="107"/>
+      <c r="P3" s="106" t="s">
         <v>7</v>
       </c>
-      <c r="Q3" s="118"/>
-      <c r="R3" s="118"/>
-      <c r="S3" s="118"/>
-      <c r="T3" s="118"/>
-      <c r="U3" s="118"/>
-      <c r="V3" s="118"/>
-      <c r="W3" s="117" t="s">
+      <c r="Q3" s="107"/>
+      <c r="R3" s="107"/>
+      <c r="S3" s="107"/>
+      <c r="T3" s="107"/>
+      <c r="U3" s="107"/>
+      <c r="V3" s="107"/>
+      <c r="W3" s="106" t="s">
         <v>8</v>
       </c>
-      <c r="X3" s="118"/>
-      <c r="Y3" s="118"/>
-      <c r="Z3" s="118"/>
-      <c r="AA3" s="118"/>
-      <c r="AB3" s="118"/>
-      <c r="AC3" s="118"/>
-      <c r="AD3" s="117" t="s">
+      <c r="X3" s="107"/>
+      <c r="Y3" s="107"/>
+      <c r="Z3" s="107"/>
+      <c r="AA3" s="107"/>
+      <c r="AB3" s="107"/>
+      <c r="AC3" s="107"/>
+      <c r="AD3" s="106" t="s">
         <v>9</v>
       </c>
-      <c r="AE3" s="118"/>
-      <c r="AF3" s="118"/>
-      <c r="AG3" s="118"/>
-      <c r="AH3" s="118"/>
-      <c r="AI3" s="118"/>
-      <c r="AJ3" s="118"/>
-      <c r="AK3" s="117" t="s">
+      <c r="AE3" s="107"/>
+      <c r="AF3" s="107"/>
+      <c r="AG3" s="107"/>
+      <c r="AH3" s="107"/>
+      <c r="AI3" s="107"/>
+      <c r="AJ3" s="107"/>
+      <c r="AK3" s="106" t="s">
         <v>10</v>
       </c>
-      <c r="AL3" s="118"/>
-      <c r="AM3" s="118"/>
-      <c r="AN3" s="118"/>
-      <c r="AO3" s="118"/>
-      <c r="AP3" s="118"/>
-      <c r="AQ3" s="118"/>
-      <c r="AR3" s="117" t="s">
+      <c r="AL3" s="107"/>
+      <c r="AM3" s="107"/>
+      <c r="AN3" s="107"/>
+      <c r="AO3" s="107"/>
+      <c r="AP3" s="107"/>
+      <c r="AQ3" s="107"/>
+      <c r="AR3" s="106" t="s">
         <v>11</v>
       </c>
-      <c r="AS3" s="118"/>
-      <c r="AT3" s="118"/>
-      <c r="AU3" s="118"/>
-      <c r="AV3" s="118"/>
-      <c r="AW3" s="118"/>
-      <c r="AX3" s="118"/>
-      <c r="AY3" s="117" t="s">
+      <c r="AS3" s="107"/>
+      <c r="AT3" s="107"/>
+      <c r="AU3" s="107"/>
+      <c r="AV3" s="107"/>
+      <c r="AW3" s="107"/>
+      <c r="AX3" s="107"/>
+      <c r="AY3" s="106" t="s">
         <v>12</v>
       </c>
-      <c r="AZ3" s="118"/>
-      <c r="BA3" s="118"/>
-      <c r="BB3" s="118"/>
-      <c r="BC3" s="118"/>
-      <c r="BD3" s="118"/>
-      <c r="BE3" s="118"/>
-      <c r="BF3" s="117" t="s">
+      <c r="AZ3" s="107"/>
+      <c r="BA3" s="107"/>
+      <c r="BB3" s="107"/>
+      <c r="BC3" s="107"/>
+      <c r="BD3" s="107"/>
+      <c r="BE3" s="107"/>
+      <c r="BF3" s="106" t="s">
         <v>13</v>
       </c>
-      <c r="BG3" s="118"/>
-      <c r="BH3" s="118"/>
-      <c r="BI3" s="118"/>
-      <c r="BJ3" s="118"/>
-      <c r="BK3" s="118"/>
-      <c r="BL3" s="118"/>
+      <c r="BG3" s="107"/>
+      <c r="BH3" s="107"/>
+      <c r="BI3" s="107"/>
+      <c r="BJ3" s="107"/>
+      <c r="BK3" s="107"/>
+      <c r="BL3" s="107"/>
     </row>
     <row r="4" spans="1:64" s="26" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="14"/>
@@ -2036,332 +2032,332 @@
         <v>14</v>
       </c>
       <c r="E4" s="30"/>
-      <c r="I4" s="117">
+      <c r="I4" s="106">
         <f ca="1">I5</f>
-        <v>45194</v>
-      </c>
-      <c r="J4" s="118"/>
-      <c r="K4" s="118"/>
-      <c r="L4" s="118"/>
-      <c r="M4" s="118"/>
-      <c r="N4" s="118"/>
-      <c r="O4" s="118"/>
-      <c r="P4" s="118">
+        <v>45201</v>
+      </c>
+      <c r="J4" s="107"/>
+      <c r="K4" s="107"/>
+      <c r="L4" s="107"/>
+      <c r="M4" s="107"/>
+      <c r="N4" s="107"/>
+      <c r="O4" s="107"/>
+      <c r="P4" s="107">
         <f ca="1">P5</f>
-        <v>45201</v>
-      </c>
-      <c r="Q4" s="118"/>
-      <c r="R4" s="118"/>
-      <c r="S4" s="118"/>
-      <c r="T4" s="118"/>
-      <c r="U4" s="118"/>
-      <c r="V4" s="118"/>
-      <c r="W4" s="118">
+        <v>45208</v>
+      </c>
+      <c r="Q4" s="107"/>
+      <c r="R4" s="107"/>
+      <c r="S4" s="107"/>
+      <c r="T4" s="107"/>
+      <c r="U4" s="107"/>
+      <c r="V4" s="107"/>
+      <c r="W4" s="107">
         <f ca="1">W5</f>
-        <v>45208</v>
-      </c>
-      <c r="X4" s="118"/>
-      <c r="Y4" s="118"/>
-      <c r="Z4" s="118"/>
-      <c r="AA4" s="118"/>
-      <c r="AB4" s="118"/>
-      <c r="AC4" s="118"/>
-      <c r="AD4" s="118">
+        <v>45215</v>
+      </c>
+      <c r="X4" s="107"/>
+      <c r="Y4" s="107"/>
+      <c r="Z4" s="107"/>
+      <c r="AA4" s="107"/>
+      <c r="AB4" s="107"/>
+      <c r="AC4" s="107"/>
+      <c r="AD4" s="107">
         <f ca="1">AD5</f>
-        <v>45215</v>
-      </c>
-      <c r="AE4" s="118"/>
-      <c r="AF4" s="118"/>
-      <c r="AG4" s="118"/>
-      <c r="AH4" s="118"/>
-      <c r="AI4" s="118"/>
-      <c r="AJ4" s="118"/>
-      <c r="AK4" s="118">
+        <v>45222</v>
+      </c>
+      <c r="AE4" s="107"/>
+      <c r="AF4" s="107"/>
+      <c r="AG4" s="107"/>
+      <c r="AH4" s="107"/>
+      <c r="AI4" s="107"/>
+      <c r="AJ4" s="107"/>
+      <c r="AK4" s="107">
         <f ca="1">AK5</f>
-        <v>45222</v>
-      </c>
-      <c r="AL4" s="118"/>
-      <c r="AM4" s="118"/>
-      <c r="AN4" s="118"/>
-      <c r="AO4" s="118"/>
-      <c r="AP4" s="118"/>
-      <c r="AQ4" s="118"/>
-      <c r="AR4" s="118">
+        <v>45229</v>
+      </c>
+      <c r="AL4" s="107"/>
+      <c r="AM4" s="107"/>
+      <c r="AN4" s="107"/>
+      <c r="AO4" s="107"/>
+      <c r="AP4" s="107"/>
+      <c r="AQ4" s="107"/>
+      <c r="AR4" s="107">
         <f ca="1">AR5</f>
-        <v>45229</v>
-      </c>
-      <c r="AS4" s="118"/>
-      <c r="AT4" s="118"/>
-      <c r="AU4" s="118"/>
-      <c r="AV4" s="118"/>
-      <c r="AW4" s="118"/>
-      <c r="AX4" s="118"/>
-      <c r="AY4" s="118">
+        <v>45236</v>
+      </c>
+      <c r="AS4" s="107"/>
+      <c r="AT4" s="107"/>
+      <c r="AU4" s="107"/>
+      <c r="AV4" s="107"/>
+      <c r="AW4" s="107"/>
+      <c r="AX4" s="107"/>
+      <c r="AY4" s="107">
         <f ca="1">AY5</f>
-        <v>45236</v>
-      </c>
-      <c r="AZ4" s="118"/>
-      <c r="BA4" s="118"/>
-      <c r="BB4" s="118"/>
-      <c r="BC4" s="118"/>
-      <c r="BD4" s="118"/>
-      <c r="BE4" s="118"/>
-      <c r="BF4" s="118">
+        <v>45243</v>
+      </c>
+      <c r="AZ4" s="107"/>
+      <c r="BA4" s="107"/>
+      <c r="BB4" s="107"/>
+      <c r="BC4" s="107"/>
+      <c r="BD4" s="107"/>
+      <c r="BE4" s="107"/>
+      <c r="BF4" s="107">
         <f ca="1">BF5</f>
-        <v>45243</v>
-      </c>
-      <c r="BG4" s="118"/>
-      <c r="BH4" s="118"/>
-      <c r="BI4" s="118"/>
-      <c r="BJ4" s="118"/>
-      <c r="BK4" s="118"/>
-      <c r="BL4" s="119"/>
+        <v>45250</v>
+      </c>
+      <c r="BG4" s="107"/>
+      <c r="BH4" s="107"/>
+      <c r="BI4" s="107"/>
+      <c r="BJ4" s="107"/>
+      <c r="BK4" s="107"/>
+      <c r="BL4" s="108"/>
     </row>
     <row r="5" spans="1:64" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="106"/>
-      <c r="B5" s="107" t="s">
+      <c r="A5" s="116"/>
+      <c r="B5" s="117" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="109" t="s">
+      <c r="C5" s="119" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="111" t="s">
+      <c r="D5" s="109" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="111" t="s">
+      <c r="E5" s="109" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="111" t="s">
+      <c r="F5" s="109" t="s">
         <v>19</v>
       </c>
       <c r="I5" s="31">
         <f ca="1">Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
-        <v>45194</v>
+        <v>45201</v>
       </c>
       <c r="J5" s="31">
         <f ca="1">I5+1</f>
-        <v>45195</v>
+        <v>45202</v>
       </c>
       <c r="K5" s="31">
         <f t="shared" ref="K5:AX5" ca="1" si="0">J5+1</f>
-        <v>45196</v>
+        <v>45203</v>
       </c>
       <c r="L5" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>45197</v>
+        <v>45204</v>
       </c>
       <c r="M5" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>45198</v>
+        <v>45205</v>
       </c>
       <c r="N5" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>45199</v>
+        <v>45206</v>
       </c>
       <c r="O5" s="32">
         <f t="shared" ca="1" si="0"/>
-        <v>45200</v>
+        <v>45207</v>
       </c>
       <c r="P5" s="33">
         <f ca="1">O5+1</f>
-        <v>45201</v>
+        <v>45208</v>
       </c>
       <c r="Q5" s="31">
         <f ca="1">P5+1</f>
-        <v>45202</v>
+        <v>45209</v>
       </c>
       <c r="R5" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>45203</v>
+        <v>45210</v>
       </c>
       <c r="S5" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>45204</v>
+        <v>45211</v>
       </c>
       <c r="T5" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>45205</v>
+        <v>45212</v>
       </c>
       <c r="U5" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>45206</v>
+        <v>45213</v>
       </c>
       <c r="V5" s="32">
         <f t="shared" ca="1" si="0"/>
-        <v>45207</v>
+        <v>45214</v>
       </c>
       <c r="W5" s="33">
         <f ca="1">V5+1</f>
-        <v>45208</v>
+        <v>45215</v>
       </c>
       <c r="X5" s="31">
         <f ca="1">W5+1</f>
-        <v>45209</v>
+        <v>45216</v>
       </c>
       <c r="Y5" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>45210</v>
+        <v>45217</v>
       </c>
       <c r="Z5" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>45211</v>
+        <v>45218</v>
       </c>
       <c r="AA5" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>45212</v>
+        <v>45219</v>
       </c>
       <c r="AB5" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>45213</v>
+        <v>45220</v>
       </c>
       <c r="AC5" s="32">
         <f t="shared" ca="1" si="0"/>
-        <v>45214</v>
+        <v>45221</v>
       </c>
       <c r="AD5" s="33">
         <f ca="1">AC5+1</f>
-        <v>45215</v>
+        <v>45222</v>
       </c>
       <c r="AE5" s="31">
         <f ca="1">AD5+1</f>
-        <v>45216</v>
+        <v>45223</v>
       </c>
       <c r="AF5" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>45217</v>
+        <v>45224</v>
       </c>
       <c r="AG5" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>45218</v>
+        <v>45225</v>
       </c>
       <c r="AH5" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>45219</v>
+        <v>45226</v>
       </c>
       <c r="AI5" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>45220</v>
+        <v>45227</v>
       </c>
       <c r="AJ5" s="32">
         <f t="shared" ca="1" si="0"/>
-        <v>45221</v>
+        <v>45228</v>
       </c>
       <c r="AK5" s="33">
         <f ca="1">AJ5+1</f>
-        <v>45222</v>
+        <v>45229</v>
       </c>
       <c r="AL5" s="31">
         <f ca="1">AK5+1</f>
-        <v>45223</v>
+        <v>45230</v>
       </c>
       <c r="AM5" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>45224</v>
+        <v>45231</v>
       </c>
       <c r="AN5" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>45225</v>
+        <v>45232</v>
       </c>
       <c r="AO5" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>45226</v>
+        <v>45233</v>
       </c>
       <c r="AP5" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>45227</v>
+        <v>45234</v>
       </c>
       <c r="AQ5" s="32">
         <f t="shared" ca="1" si="0"/>
-        <v>45228</v>
+        <v>45235</v>
       </c>
       <c r="AR5" s="33">
         <f ca="1">AQ5+1</f>
-        <v>45229</v>
+        <v>45236</v>
       </c>
       <c r="AS5" s="31">
         <f ca="1">AR5+1</f>
-        <v>45230</v>
+        <v>45237</v>
       </c>
       <c r="AT5" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>45231</v>
+        <v>45238</v>
       </c>
       <c r="AU5" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>45232</v>
+        <v>45239</v>
       </c>
       <c r="AV5" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>45233</v>
+        <v>45240</v>
       </c>
       <c r="AW5" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>45234</v>
+        <v>45241</v>
       </c>
       <c r="AX5" s="32">
         <f t="shared" ca="1" si="0"/>
-        <v>45235</v>
+        <v>45242</v>
       </c>
       <c r="AY5" s="33">
         <f ca="1">AX5+1</f>
-        <v>45236</v>
+        <v>45243</v>
       </c>
       <c r="AZ5" s="31">
         <f ca="1">AY5+1</f>
-        <v>45237</v>
+        <v>45244</v>
       </c>
       <c r="BA5" s="31">
         <f t="shared" ref="BA5:BE5" ca="1" si="1">AZ5+1</f>
-        <v>45238</v>
+        <v>45245</v>
       </c>
       <c r="BB5" s="31">
         <f t="shared" ca="1" si="1"/>
-        <v>45239</v>
+        <v>45246</v>
       </c>
       <c r="BC5" s="31">
         <f t="shared" ca="1" si="1"/>
-        <v>45240</v>
+        <v>45247</v>
       </c>
       <c r="BD5" s="31">
         <f t="shared" ca="1" si="1"/>
-        <v>45241</v>
+        <v>45248</v>
       </c>
       <c r="BE5" s="32">
         <f t="shared" ca="1" si="1"/>
-        <v>45242</v>
+        <v>45249</v>
       </c>
       <c r="BF5" s="33">
         <f ca="1">BE5+1</f>
-        <v>45243</v>
+        <v>45250</v>
       </c>
       <c r="BG5" s="31">
         <f ca="1">BF5+1</f>
-        <v>45244</v>
+        <v>45251</v>
       </c>
       <c r="BH5" s="31">
         <f t="shared" ref="BH5:BL5" ca="1" si="2">BG5+1</f>
-        <v>45245</v>
+        <v>45252</v>
       </c>
       <c r="BI5" s="31">
         <f t="shared" ca="1" si="2"/>
-        <v>45246</v>
+        <v>45253</v>
       </c>
       <c r="BJ5" s="31">
         <f t="shared" ca="1" si="2"/>
-        <v>45247</v>
+        <v>45254</v>
       </c>
       <c r="BK5" s="31">
         <f t="shared" ca="1" si="2"/>
-        <v>45248</v>
+        <v>45255</v>
       </c>
       <c r="BL5" s="31">
         <f t="shared" ca="1" si="2"/>
-        <v>45249</v>
+        <v>45256</v>
       </c>
     </row>
     <row r="6" spans="1:64" s="26" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="106"/>
-      <c r="B6" s="108"/>
+      <c r="A6" s="116"/>
+      <c r="B6" s="118"/>
       <c r="C6" s="110"/>
       <c r="D6" s="110"/>
       <c r="E6" s="110"/>
@@ -2740,14 +2736,16 @@
       <c r="C9" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="49"/>
+      <c r="D9" s="49">
+        <v>1</v>
+      </c>
       <c r="E9" s="50">
         <f ca="1">Project_Start</f>
-        <v>45195</v>
+        <v>45204</v>
       </c>
       <c r="F9" s="50">
         <f ca="1">E9+3</f>
-        <v>45198</v>
+        <v>45207</v>
       </c>
       <c r="G9" s="17"/>
       <c r="H9" s="5">
@@ -2819,14 +2817,16 @@
       <c r="C10" s="53" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="54"/>
+      <c r="D10" s="54">
+        <v>0.85</v>
+      </c>
       <c r="E10" s="50">
         <f ca="1">Project_Start</f>
-        <v>45195</v>
+        <v>45204</v>
       </c>
       <c r="F10" s="50">
         <f ca="1">E10+3</f>
-        <v>45198</v>
+        <v>45207</v>
       </c>
       <c r="G10" s="17"/>
       <c r="H10" s="5">
@@ -2898,14 +2898,16 @@
       <c r="C11" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="54"/>
+      <c r="D11" s="54">
+        <v>1</v>
+      </c>
       <c r="E11" s="55">
         <f ca="1">F10</f>
-        <v>45198</v>
+        <v>45207</v>
       </c>
       <c r="F11" s="55">
         <f ca="1">E11+4</f>
-        <v>45202</v>
+        <v>45211</v>
       </c>
       <c r="G11" s="17"/>
       <c r="H11" s="5">
@@ -2977,14 +2979,16 @@
       <c r="C12" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="54"/>
+      <c r="D12" s="54">
+        <v>1</v>
+      </c>
       <c r="E12" s="55">
         <f ca="1">F11</f>
-        <v>45202</v>
+        <v>45211</v>
       </c>
       <c r="F12" s="55">
         <f ca="1">E12+2</f>
-        <v>45204</v>
+        <v>45213</v>
       </c>
       <c r="G12" s="17"/>
       <c r="H12" s="5">
@@ -3056,7 +3060,9 @@
       <c r="C13" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="54"/>
+      <c r="D13" s="54">
+        <v>1</v>
+      </c>
       <c r="E13" s="55">
         <v>45204</v>
       </c>
@@ -3617,11 +3623,11 @@
       <c r="D21" s="74"/>
       <c r="E21" s="75">
         <f ca="1">E9+15</f>
-        <v>45210</v>
+        <v>45219</v>
       </c>
       <c r="F21" s="75">
         <f ca="1">E21+5</f>
-        <v>45215</v>
+        <v>45224</v>
       </c>
       <c r="G21" s="17"/>
       <c r="H21" s="5">
@@ -4610,11 +4616,19 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="AD3:AJ3"/>
-    <mergeCell ref="AK3:AQ3"/>
-    <mergeCell ref="AR3:AX3"/>
-    <mergeCell ref="AY3:BE3"/>
-    <mergeCell ref="BF3:BL3"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="Q2:Z2"/>
+    <mergeCell ref="Q1:Z1"/>
+    <mergeCell ref="I1:O1"/>
+    <mergeCell ref="I2:O2"/>
+    <mergeCell ref="I3:O3"/>
+    <mergeCell ref="P3:V3"/>
+    <mergeCell ref="W3:AC3"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="I4:O4"/>
     <mergeCell ref="P4:V4"/>
@@ -4623,19 +4637,11 @@
     <mergeCell ref="AK4:AQ4"/>
     <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="AY4:BE4"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="Q2:Z2"/>
-    <mergeCell ref="Q1:Z1"/>
-    <mergeCell ref="I1:O1"/>
-    <mergeCell ref="I2:O2"/>
-    <mergeCell ref="I3:O3"/>
-    <mergeCell ref="P3:V3"/>
-    <mergeCell ref="W3:AC3"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="AD3:AJ3"/>
+    <mergeCell ref="AK3:AQ3"/>
+    <mergeCell ref="AR3:AX3"/>
+    <mergeCell ref="AY3:BE3"/>
+    <mergeCell ref="BF3:BL3"/>
   </mergeCells>
   <phoneticPr fontId="32" type="noConversion"/>
   <conditionalFormatting sqref="D7:D33">
@@ -4899,6 +4905,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F010965E38DD9C4C9BE78EF37B7A5F63" ma:contentTypeVersion="3" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6e5a01bfcf6a1a5eee5a5ca1585b5a1a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="3e43f44c-3f4d-46ba-91a0-7c8ec4d7a2ca" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="00e6d9bda136d3704b372a6b2e4b23e5" ns3:_="">
     <xsd:import namespace="3e43f44c-3f4d-46ba-91a0-7c8ec4d7a2ca"/>
@@ -5036,22 +5057,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A82239A0-E68C-493F-BEE6-C77FEA397FD6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="3e43f44c-3f4d-46ba-91a0-7c8ec4d7a2ca"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A800D70D-3EC9-4DB9-B9D8-9E383CE8B438}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5069,30 +5099,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A82239A0-E68C-493F-BEE6-C77FEA397FD6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="3e43f44c-3f4d-46ba-91a0-7c8ec4d7a2ca"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata"/>
 </file>
</xml_diff>

<commit_message>
Updated the Gantt Chart
adjusted how far along the milestones we have accomplished
</commit_message>
<xml_diff>
--- a/Project Spyn Gantt Chart.xlsx
+++ b/Project Spyn Gantt Chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tydng\Desktop\FSE-100-Team-4-Sheibanian\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49679D53-7A36-4A85-B6EF-7613B86E3018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D61AF071-C535-4150-9ED9-568683C9E2CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1136,19 +1136,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="1"/>
     </xf>
-    <xf numFmtId="166" fontId="19" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="19" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="19" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1160,17 +1163,14 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="166" fontId="19" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="19" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="19" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -1862,8 +1862,8 @@
   </sheetPr>
   <dimension ref="A1:BL36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="B1" zoomScale="115" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A5" zoomScale="81" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1889,29 +1889,29 @@
       <c r="E1" s="20"/>
       <c r="F1" s="21"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="114" t="s">
+      <c r="I1" s="115" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="115"/>
-      <c r="K1" s="115"/>
-      <c r="L1" s="115"/>
-      <c r="M1" s="115"/>
-      <c r="N1" s="115"/>
-      <c r="O1" s="115"/>
+      <c r="J1" s="116"/>
+      <c r="K1" s="116"/>
+      <c r="L1" s="116"/>
+      <c r="M1" s="116"/>
+      <c r="N1" s="116"/>
+      <c r="O1" s="116"/>
       <c r="P1" s="24"/>
-      <c r="Q1" s="113">
+      <c r="Q1" s="114">
         <f ca="1">TODAY()</f>
-        <v>45204</v>
-      </c>
-      <c r="R1" s="112"/>
-      <c r="S1" s="112"/>
-      <c r="T1" s="112"/>
-      <c r="U1" s="112"/>
-      <c r="V1" s="112"/>
-      <c r="W1" s="112"/>
-      <c r="X1" s="112"/>
-      <c r="Y1" s="112"/>
-      <c r="Z1" s="112"/>
+        <v>45211</v>
+      </c>
+      <c r="R1" s="113"/>
+      <c r="S1" s="113"/>
+      <c r="T1" s="113"/>
+      <c r="U1" s="113"/>
+      <c r="V1" s="113"/>
+      <c r="W1" s="113"/>
+      <c r="X1" s="113"/>
+      <c r="Y1" s="113"/>
+      <c r="Z1" s="113"/>
     </row>
     <row r="2" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B2" s="96" t="s">
@@ -1923,28 +1923,28 @@
       <c r="D2" s="22"/>
       <c r="E2" s="23"/>
       <c r="F2" s="22"/>
-      <c r="I2" s="114" t="s">
+      <c r="I2" s="115" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="115"/>
-      <c r="K2" s="115"/>
-      <c r="L2" s="115"/>
-      <c r="M2" s="115"/>
-      <c r="N2" s="115"/>
-      <c r="O2" s="115"/>
+      <c r="J2" s="116"/>
+      <c r="K2" s="116"/>
+      <c r="L2" s="116"/>
+      <c r="M2" s="116"/>
+      <c r="N2" s="116"/>
+      <c r="O2" s="116"/>
       <c r="P2" s="24"/>
-      <c r="Q2" s="111">
+      <c r="Q2" s="112">
         <v>1</v>
       </c>
-      <c r="R2" s="112"/>
-      <c r="S2" s="112"/>
-      <c r="T2" s="112"/>
-      <c r="U2" s="112"/>
-      <c r="V2" s="112"/>
-      <c r="W2" s="112"/>
-      <c r="X2" s="112"/>
-      <c r="Y2" s="112"/>
-      <c r="Z2" s="112"/>
+      <c r="R2" s="113"/>
+      <c r="S2" s="113"/>
+      <c r="T2" s="113"/>
+      <c r="U2" s="113"/>
+      <c r="V2" s="113"/>
+      <c r="W2" s="113"/>
+      <c r="X2" s="113"/>
+      <c r="Y2" s="113"/>
+      <c r="Z2" s="113"/>
     </row>
     <row r="3" spans="1:64" s="26" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13"/>
@@ -1953,78 +1953,78 @@
       </c>
       <c r="D3" s="27"/>
       <c r="E3" s="28"/>
-      <c r="I3" s="106" t="s">
+      <c r="I3" s="117" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="107"/>
-      <c r="K3" s="107"/>
-      <c r="L3" s="107"/>
-      <c r="M3" s="107"/>
-      <c r="N3" s="107"/>
-      <c r="O3" s="107"/>
-      <c r="P3" s="106" t="s">
+      <c r="J3" s="118"/>
+      <c r="K3" s="118"/>
+      <c r="L3" s="118"/>
+      <c r="M3" s="118"/>
+      <c r="N3" s="118"/>
+      <c r="O3" s="118"/>
+      <c r="P3" s="117" t="s">
         <v>7</v>
       </c>
-      <c r="Q3" s="107"/>
-      <c r="R3" s="107"/>
-      <c r="S3" s="107"/>
-      <c r="T3" s="107"/>
-      <c r="U3" s="107"/>
-      <c r="V3" s="107"/>
-      <c r="W3" s="106" t="s">
+      <c r="Q3" s="118"/>
+      <c r="R3" s="118"/>
+      <c r="S3" s="118"/>
+      <c r="T3" s="118"/>
+      <c r="U3" s="118"/>
+      <c r="V3" s="118"/>
+      <c r="W3" s="117" t="s">
         <v>8</v>
       </c>
-      <c r="X3" s="107"/>
-      <c r="Y3" s="107"/>
-      <c r="Z3" s="107"/>
-      <c r="AA3" s="107"/>
-      <c r="AB3" s="107"/>
-      <c r="AC3" s="107"/>
-      <c r="AD3" s="106" t="s">
+      <c r="X3" s="118"/>
+      <c r="Y3" s="118"/>
+      <c r="Z3" s="118"/>
+      <c r="AA3" s="118"/>
+      <c r="AB3" s="118"/>
+      <c r="AC3" s="118"/>
+      <c r="AD3" s="117" t="s">
         <v>9</v>
       </c>
-      <c r="AE3" s="107"/>
-      <c r="AF3" s="107"/>
-      <c r="AG3" s="107"/>
-      <c r="AH3" s="107"/>
-      <c r="AI3" s="107"/>
-      <c r="AJ3" s="107"/>
-      <c r="AK3" s="106" t="s">
+      <c r="AE3" s="118"/>
+      <c r="AF3" s="118"/>
+      <c r="AG3" s="118"/>
+      <c r="AH3" s="118"/>
+      <c r="AI3" s="118"/>
+      <c r="AJ3" s="118"/>
+      <c r="AK3" s="117" t="s">
         <v>10</v>
       </c>
-      <c r="AL3" s="107"/>
-      <c r="AM3" s="107"/>
-      <c r="AN3" s="107"/>
-      <c r="AO3" s="107"/>
-      <c r="AP3" s="107"/>
-      <c r="AQ3" s="107"/>
-      <c r="AR3" s="106" t="s">
+      <c r="AL3" s="118"/>
+      <c r="AM3" s="118"/>
+      <c r="AN3" s="118"/>
+      <c r="AO3" s="118"/>
+      <c r="AP3" s="118"/>
+      <c r="AQ3" s="118"/>
+      <c r="AR3" s="117" t="s">
         <v>11</v>
       </c>
-      <c r="AS3" s="107"/>
-      <c r="AT3" s="107"/>
-      <c r="AU3" s="107"/>
-      <c r="AV3" s="107"/>
-      <c r="AW3" s="107"/>
-      <c r="AX3" s="107"/>
-      <c r="AY3" s="106" t="s">
+      <c r="AS3" s="118"/>
+      <c r="AT3" s="118"/>
+      <c r="AU3" s="118"/>
+      <c r="AV3" s="118"/>
+      <c r="AW3" s="118"/>
+      <c r="AX3" s="118"/>
+      <c r="AY3" s="117" t="s">
         <v>12</v>
       </c>
-      <c r="AZ3" s="107"/>
-      <c r="BA3" s="107"/>
-      <c r="BB3" s="107"/>
-      <c r="BC3" s="107"/>
-      <c r="BD3" s="107"/>
-      <c r="BE3" s="107"/>
-      <c r="BF3" s="106" t="s">
+      <c r="AZ3" s="118"/>
+      <c r="BA3" s="118"/>
+      <c r="BB3" s="118"/>
+      <c r="BC3" s="118"/>
+      <c r="BD3" s="118"/>
+      <c r="BE3" s="118"/>
+      <c r="BF3" s="117" t="s">
         <v>13</v>
       </c>
-      <c r="BG3" s="107"/>
-      <c r="BH3" s="107"/>
-      <c r="BI3" s="107"/>
-      <c r="BJ3" s="107"/>
-      <c r="BK3" s="107"/>
-      <c r="BL3" s="107"/>
+      <c r="BG3" s="118"/>
+      <c r="BH3" s="118"/>
+      <c r="BI3" s="118"/>
+      <c r="BJ3" s="118"/>
+      <c r="BK3" s="118"/>
+      <c r="BL3" s="118"/>
     </row>
     <row r="4" spans="1:64" s="26" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="14"/>
@@ -2032,332 +2032,332 @@
         <v>14</v>
       </c>
       <c r="E4" s="30"/>
-      <c r="I4" s="106">
+      <c r="I4" s="117">
         <f ca="1">I5</f>
-        <v>45201</v>
-      </c>
-      <c r="J4" s="107"/>
-      <c r="K4" s="107"/>
-      <c r="L4" s="107"/>
-      <c r="M4" s="107"/>
-      <c r="N4" s="107"/>
-      <c r="O4" s="107"/>
-      <c r="P4" s="107">
+        <v>45208</v>
+      </c>
+      <c r="J4" s="118"/>
+      <c r="K4" s="118"/>
+      <c r="L4" s="118"/>
+      <c r="M4" s="118"/>
+      <c r="N4" s="118"/>
+      <c r="O4" s="118"/>
+      <c r="P4" s="118">
         <f ca="1">P5</f>
-        <v>45208</v>
-      </c>
-      <c r="Q4" s="107"/>
-      <c r="R4" s="107"/>
-      <c r="S4" s="107"/>
-      <c r="T4" s="107"/>
-      <c r="U4" s="107"/>
-      <c r="V4" s="107"/>
-      <c r="W4" s="107">
+        <v>45215</v>
+      </c>
+      <c r="Q4" s="118"/>
+      <c r="R4" s="118"/>
+      <c r="S4" s="118"/>
+      <c r="T4" s="118"/>
+      <c r="U4" s="118"/>
+      <c r="V4" s="118"/>
+      <c r="W4" s="118">
         <f ca="1">W5</f>
-        <v>45215</v>
-      </c>
-      <c r="X4" s="107"/>
-      <c r="Y4" s="107"/>
-      <c r="Z4" s="107"/>
-      <c r="AA4" s="107"/>
-      <c r="AB4" s="107"/>
-      <c r="AC4" s="107"/>
-      <c r="AD4" s="107">
+        <v>45222</v>
+      </c>
+      <c r="X4" s="118"/>
+      <c r="Y4" s="118"/>
+      <c r="Z4" s="118"/>
+      <c r="AA4" s="118"/>
+      <c r="AB4" s="118"/>
+      <c r="AC4" s="118"/>
+      <c r="AD4" s="118">
         <f ca="1">AD5</f>
-        <v>45222</v>
-      </c>
-      <c r="AE4" s="107"/>
-      <c r="AF4" s="107"/>
-      <c r="AG4" s="107"/>
-      <c r="AH4" s="107"/>
-      <c r="AI4" s="107"/>
-      <c r="AJ4" s="107"/>
-      <c r="AK4" s="107">
+        <v>45229</v>
+      </c>
+      <c r="AE4" s="118"/>
+      <c r="AF4" s="118"/>
+      <c r="AG4" s="118"/>
+      <c r="AH4" s="118"/>
+      <c r="AI4" s="118"/>
+      <c r="AJ4" s="118"/>
+      <c r="AK4" s="118">
         <f ca="1">AK5</f>
-        <v>45229</v>
-      </c>
-      <c r="AL4" s="107"/>
-      <c r="AM4" s="107"/>
-      <c r="AN4" s="107"/>
-      <c r="AO4" s="107"/>
-      <c r="AP4" s="107"/>
-      <c r="AQ4" s="107"/>
-      <c r="AR4" s="107">
+        <v>45236</v>
+      </c>
+      <c r="AL4" s="118"/>
+      <c r="AM4" s="118"/>
+      <c r="AN4" s="118"/>
+      <c r="AO4" s="118"/>
+      <c r="AP4" s="118"/>
+      <c r="AQ4" s="118"/>
+      <c r="AR4" s="118">
         <f ca="1">AR5</f>
-        <v>45236</v>
-      </c>
-      <c r="AS4" s="107"/>
-      <c r="AT4" s="107"/>
-      <c r="AU4" s="107"/>
-      <c r="AV4" s="107"/>
-      <c r="AW4" s="107"/>
-      <c r="AX4" s="107"/>
-      <c r="AY4" s="107">
+        <v>45243</v>
+      </c>
+      <c r="AS4" s="118"/>
+      <c r="AT4" s="118"/>
+      <c r="AU4" s="118"/>
+      <c r="AV4" s="118"/>
+      <c r="AW4" s="118"/>
+      <c r="AX4" s="118"/>
+      <c r="AY4" s="118">
         <f ca="1">AY5</f>
-        <v>45243</v>
-      </c>
-      <c r="AZ4" s="107"/>
-      <c r="BA4" s="107"/>
-      <c r="BB4" s="107"/>
-      <c r="BC4" s="107"/>
-      <c r="BD4" s="107"/>
-      <c r="BE4" s="107"/>
-      <c r="BF4" s="107">
+        <v>45250</v>
+      </c>
+      <c r="AZ4" s="118"/>
+      <c r="BA4" s="118"/>
+      <c r="BB4" s="118"/>
+      <c r="BC4" s="118"/>
+      <c r="BD4" s="118"/>
+      <c r="BE4" s="118"/>
+      <c r="BF4" s="118">
         <f ca="1">BF5</f>
-        <v>45250</v>
-      </c>
-      <c r="BG4" s="107"/>
-      <c r="BH4" s="107"/>
-      <c r="BI4" s="107"/>
-      <c r="BJ4" s="107"/>
-      <c r="BK4" s="107"/>
-      <c r="BL4" s="108"/>
+        <v>45257</v>
+      </c>
+      <c r="BG4" s="118"/>
+      <c r="BH4" s="118"/>
+      <c r="BI4" s="118"/>
+      <c r="BJ4" s="118"/>
+      <c r="BK4" s="118"/>
+      <c r="BL4" s="119"/>
     </row>
     <row r="5" spans="1:64" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="116"/>
-      <c r="B5" s="117" t="s">
+      <c r="A5" s="106"/>
+      <c r="B5" s="107" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="119" t="s">
+      <c r="C5" s="109" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="109" t="s">
+      <c r="D5" s="111" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="109" t="s">
+      <c r="E5" s="111" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="109" t="s">
+      <c r="F5" s="111" t="s">
         <v>19</v>
       </c>
       <c r="I5" s="31">
         <f ca="1">Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
-        <v>45201</v>
+        <v>45208</v>
       </c>
       <c r="J5" s="31">
         <f ca="1">I5+1</f>
-        <v>45202</v>
+        <v>45209</v>
       </c>
       <c r="K5" s="31">
         <f t="shared" ref="K5:AX5" ca="1" si="0">J5+1</f>
-        <v>45203</v>
+        <v>45210</v>
       </c>
       <c r="L5" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>45204</v>
+        <v>45211</v>
       </c>
       <c r="M5" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>45205</v>
+        <v>45212</v>
       </c>
       <c r="N5" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>45206</v>
+        <v>45213</v>
       </c>
       <c r="O5" s="32">
         <f t="shared" ca="1" si="0"/>
-        <v>45207</v>
+        <v>45214</v>
       </c>
       <c r="P5" s="33">
         <f ca="1">O5+1</f>
-        <v>45208</v>
+        <v>45215</v>
       </c>
       <c r="Q5" s="31">
         <f ca="1">P5+1</f>
-        <v>45209</v>
+        <v>45216</v>
       </c>
       <c r="R5" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>45210</v>
+        <v>45217</v>
       </c>
       <c r="S5" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>45211</v>
+        <v>45218</v>
       </c>
       <c r="T5" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>45212</v>
+        <v>45219</v>
       </c>
       <c r="U5" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>45213</v>
+        <v>45220</v>
       </c>
       <c r="V5" s="32">
         <f t="shared" ca="1" si="0"/>
-        <v>45214</v>
+        <v>45221</v>
       </c>
       <c r="W5" s="33">
         <f ca="1">V5+1</f>
-        <v>45215</v>
+        <v>45222</v>
       </c>
       <c r="X5" s="31">
         <f ca="1">W5+1</f>
-        <v>45216</v>
+        <v>45223</v>
       </c>
       <c r="Y5" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>45217</v>
+        <v>45224</v>
       </c>
       <c r="Z5" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>45218</v>
+        <v>45225</v>
       </c>
       <c r="AA5" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>45219</v>
+        <v>45226</v>
       </c>
       <c r="AB5" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>45220</v>
+        <v>45227</v>
       </c>
       <c r="AC5" s="32">
         <f t="shared" ca="1" si="0"/>
-        <v>45221</v>
+        <v>45228</v>
       </c>
       <c r="AD5" s="33">
         <f ca="1">AC5+1</f>
-        <v>45222</v>
+        <v>45229</v>
       </c>
       <c r="AE5" s="31">
         <f ca="1">AD5+1</f>
-        <v>45223</v>
+        <v>45230</v>
       </c>
       <c r="AF5" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>45224</v>
+        <v>45231</v>
       </c>
       <c r="AG5" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>45225</v>
+        <v>45232</v>
       </c>
       <c r="AH5" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>45226</v>
+        <v>45233</v>
       </c>
       <c r="AI5" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>45227</v>
+        <v>45234</v>
       </c>
       <c r="AJ5" s="32">
         <f t="shared" ca="1" si="0"/>
-        <v>45228</v>
+        <v>45235</v>
       </c>
       <c r="AK5" s="33">
         <f ca="1">AJ5+1</f>
-        <v>45229</v>
+        <v>45236</v>
       </c>
       <c r="AL5" s="31">
         <f ca="1">AK5+1</f>
-        <v>45230</v>
+        <v>45237</v>
       </c>
       <c r="AM5" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>45231</v>
+        <v>45238</v>
       </c>
       <c r="AN5" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>45232</v>
+        <v>45239</v>
       </c>
       <c r="AO5" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>45233</v>
+        <v>45240</v>
       </c>
       <c r="AP5" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>45234</v>
+        <v>45241</v>
       </c>
       <c r="AQ5" s="32">
         <f t="shared" ca="1" si="0"/>
-        <v>45235</v>
+        <v>45242</v>
       </c>
       <c r="AR5" s="33">
         <f ca="1">AQ5+1</f>
-        <v>45236</v>
+        <v>45243</v>
       </c>
       <c r="AS5" s="31">
         <f ca="1">AR5+1</f>
-        <v>45237</v>
+        <v>45244</v>
       </c>
       <c r="AT5" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>45238</v>
+        <v>45245</v>
       </c>
       <c r="AU5" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>45239</v>
+        <v>45246</v>
       </c>
       <c r="AV5" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>45240</v>
+        <v>45247</v>
       </c>
       <c r="AW5" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>45241</v>
+        <v>45248</v>
       </c>
       <c r="AX5" s="32">
         <f t="shared" ca="1" si="0"/>
-        <v>45242</v>
+        <v>45249</v>
       </c>
       <c r="AY5" s="33">
         <f ca="1">AX5+1</f>
-        <v>45243</v>
+        <v>45250</v>
       </c>
       <c r="AZ5" s="31">
         <f ca="1">AY5+1</f>
-        <v>45244</v>
+        <v>45251</v>
       </c>
       <c r="BA5" s="31">
         <f t="shared" ref="BA5:BE5" ca="1" si="1">AZ5+1</f>
-        <v>45245</v>
+        <v>45252</v>
       </c>
       <c r="BB5" s="31">
         <f t="shared" ca="1" si="1"/>
-        <v>45246</v>
+        <v>45253</v>
       </c>
       <c r="BC5" s="31">
         <f t="shared" ca="1" si="1"/>
-        <v>45247</v>
+        <v>45254</v>
       </c>
       <c r="BD5" s="31">
         <f t="shared" ca="1" si="1"/>
-        <v>45248</v>
+        <v>45255</v>
       </c>
       <c r="BE5" s="32">
         <f t="shared" ca="1" si="1"/>
-        <v>45249</v>
+        <v>45256</v>
       </c>
       <c r="BF5" s="33">
         <f ca="1">BE5+1</f>
-        <v>45250</v>
+        <v>45257</v>
       </c>
       <c r="BG5" s="31">
         <f ca="1">BF5+1</f>
-        <v>45251</v>
+        <v>45258</v>
       </c>
       <c r="BH5" s="31">
         <f t="shared" ref="BH5:BL5" ca="1" si="2">BG5+1</f>
-        <v>45252</v>
+        <v>45259</v>
       </c>
       <c r="BI5" s="31">
         <f t="shared" ca="1" si="2"/>
-        <v>45253</v>
+        <v>45260</v>
       </c>
       <c r="BJ5" s="31">
         <f t="shared" ca="1" si="2"/>
-        <v>45254</v>
+        <v>45261</v>
       </c>
       <c r="BK5" s="31">
         <f t="shared" ca="1" si="2"/>
-        <v>45255</v>
+        <v>45262</v>
       </c>
       <c r="BL5" s="31">
         <f t="shared" ca="1" si="2"/>
-        <v>45256</v>
+        <v>45263</v>
       </c>
     </row>
     <row r="6" spans="1:64" s="26" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="116"/>
-      <c r="B6" s="118"/>
+      <c r="A6" s="106"/>
+      <c r="B6" s="108"/>
       <c r="C6" s="110"/>
       <c r="D6" s="110"/>
       <c r="E6" s="110"/>
@@ -2741,11 +2741,11 @@
       </c>
       <c r="E9" s="50">
         <f ca="1">Project_Start</f>
-        <v>45204</v>
+        <v>45211</v>
       </c>
       <c r="F9" s="50">
         <f ca="1">E9+3</f>
-        <v>45207</v>
+        <v>45214</v>
       </c>
       <c r="G9" s="17"/>
       <c r="H9" s="5">
@@ -2818,15 +2818,15 @@
         <v>24</v>
       </c>
       <c r="D10" s="54">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="E10" s="50">
         <f ca="1">Project_Start</f>
-        <v>45204</v>
+        <v>45211</v>
       </c>
       <c r="F10" s="50">
         <f ca="1">E10+3</f>
-        <v>45207</v>
+        <v>45214</v>
       </c>
       <c r="G10" s="17"/>
       <c r="H10" s="5">
@@ -2903,11 +2903,11 @@
       </c>
       <c r="E11" s="55">
         <f ca="1">F10</f>
-        <v>45207</v>
+        <v>45214</v>
       </c>
       <c r="F11" s="55">
         <f ca="1">E11+4</f>
-        <v>45211</v>
+        <v>45218</v>
       </c>
       <c r="G11" s="17"/>
       <c r="H11" s="5">
@@ -2984,11 +2984,11 @@
       </c>
       <c r="E12" s="55">
         <f ca="1">F11</f>
-        <v>45211</v>
+        <v>45218</v>
       </c>
       <c r="F12" s="55">
         <f ca="1">E12+2</f>
-        <v>45213</v>
+        <v>45220</v>
       </c>
       <c r="G12" s="17"/>
       <c r="H12" s="5">
@@ -3155,19 +3155,21 @@
       <c r="C15" s="63" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="64"/>
+      <c r="D15" s="64">
+        <v>0.7</v>
+      </c>
       <c r="E15" s="65">
-        <f>E13+1</f>
-        <v>45205</v>
+        <f>E13+7</f>
+        <v>45211</v>
       </c>
       <c r="F15" s="65">
-        <f>E15+4</f>
-        <v>45209</v>
+        <f>E15+3</f>
+        <v>45214</v>
       </c>
       <c r="G15" s="17"/>
       <c r="H15" s="5">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I15" s="51"/>
       <c r="J15" s="51"/>
@@ -3234,18 +3236,20 @@
       <c r="C16" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="D16" s="64"/>
+      <c r="D16" s="64">
+        <v>1</v>
+      </c>
       <c r="E16" s="65">
-        <v>45205</v>
+        <v>45211</v>
       </c>
       <c r="F16" s="65">
-        <f>E16+5</f>
-        <v>45210</v>
+        <f>E16-3</f>
+        <v>45208</v>
       </c>
       <c r="G16" s="17"/>
       <c r="H16" s="5">
         <f t="shared" si="5"/>
-        <v>6</v>
+        <v>-2</v>
       </c>
       <c r="I16" s="51"/>
       <c r="J16" s="51"/>
@@ -3312,14 +3316,16 @@
       <c r="C17" s="63" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="64"/>
+      <c r="D17" s="64">
+        <v>0.5</v>
+      </c>
       <c r="E17" s="65">
-        <f>F16</f>
-        <v>45210</v>
+        <f>E15</f>
+        <v>45211</v>
       </c>
       <c r="F17" s="65">
         <f>E17+3</f>
-        <v>45213</v>
+        <v>45214</v>
       </c>
       <c r="G17" s="17"/>
       <c r="H17" s="5">
@@ -3391,19 +3397,21 @@
       <c r="C18" s="63" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="64"/>
+      <c r="D18" s="64">
+        <v>1</v>
+      </c>
       <c r="E18" s="65">
         <f>E17</f>
-        <v>45210</v>
+        <v>45211</v>
       </c>
       <c r="F18" s="65">
-        <f>E18+2</f>
-        <v>45212</v>
+        <f>E18</f>
+        <v>45211</v>
       </c>
       <c r="G18" s="17"/>
       <c r="H18" s="5">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I18" s="51"/>
       <c r="J18" s="51"/>
@@ -3470,14 +3478,16 @@
       <c r="C19" s="63" t="s">
         <v>30</v>
       </c>
-      <c r="D19" s="64"/>
+      <c r="D19" s="64">
+        <v>0.9</v>
+      </c>
       <c r="E19" s="65">
         <f>E18</f>
-        <v>45210</v>
+        <v>45211</v>
       </c>
       <c r="F19" s="65">
         <f>E19+3</f>
-        <v>45213</v>
+        <v>45214</v>
       </c>
       <c r="G19" s="17"/>
       <c r="H19" s="5">
@@ -3623,11 +3633,11 @@
       <c r="D21" s="74"/>
       <c r="E21" s="75">
         <f ca="1">E9+15</f>
-        <v>45219</v>
+        <v>45226</v>
       </c>
       <c r="F21" s="75">
         <f ca="1">E21+5</f>
-        <v>45224</v>
+        <v>45231</v>
       </c>
       <c r="G21" s="17"/>
       <c r="H21" s="5">
@@ -4616,11 +4626,19 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="AD3:AJ3"/>
+    <mergeCell ref="AK3:AQ3"/>
+    <mergeCell ref="AR3:AX3"/>
+    <mergeCell ref="AY3:BE3"/>
+    <mergeCell ref="BF3:BL3"/>
+    <mergeCell ref="BF4:BL4"/>
+    <mergeCell ref="I4:O4"/>
+    <mergeCell ref="P4:V4"/>
+    <mergeCell ref="W4:AC4"/>
+    <mergeCell ref="AD4:AJ4"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
+    <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="F5:F6"/>
     <mergeCell ref="Q2:Z2"/>
     <mergeCell ref="Q1:Z1"/>
@@ -4629,19 +4647,11 @@
     <mergeCell ref="I3:O3"/>
     <mergeCell ref="P3:V3"/>
     <mergeCell ref="W3:AC3"/>
-    <mergeCell ref="BF4:BL4"/>
-    <mergeCell ref="I4:O4"/>
-    <mergeCell ref="P4:V4"/>
-    <mergeCell ref="W4:AC4"/>
-    <mergeCell ref="AD4:AJ4"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
-    <mergeCell ref="AY4:BE4"/>
-    <mergeCell ref="AD3:AJ3"/>
-    <mergeCell ref="AK3:AQ3"/>
-    <mergeCell ref="AR3:AX3"/>
-    <mergeCell ref="AY3:BE3"/>
-    <mergeCell ref="BF3:BL3"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
   </mergeCells>
   <phoneticPr fontId="32" type="noConversion"/>
   <conditionalFormatting sqref="D7:D33">
@@ -4754,7 +4764,7 @@
     <oddFooter>Page &amp;P of &amp;N</oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="F18 F28" formula="1"/>
+    <ignoredError sqref="F28" formula="1"/>
   </ignoredErrors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
@@ -4911,15 +4921,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F010965E38DD9C4C9BE78EF37B7A5F63" ma:contentTypeVersion="3" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6e5a01bfcf6a1a5eee5a5ca1585b5a1a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="3e43f44c-3f4d-46ba-91a0-7c8ec4d7a2ca" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="00e6d9bda136d3704b372a6b2e4b23e5" ns3:_="">
     <xsd:import namespace="3e43f44c-3f4d-46ba-91a0-7c8ec4d7a2ca"/>
@@ -5057,6 +5058,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A82239A0-E68C-493F-BEE6-C77FEA397FD6}">
   <ds:schemaRefs>
@@ -5074,14 +5084,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A800D70D-3EC9-4DB9-B9D8-9E383CE8B438}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5099,6 +5101,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata"/>
 </file>
</xml_diff>

<commit_message>
Updated again to fix mistakes
</commit_message>
<xml_diff>
--- a/Project Spyn Gantt Chart.xlsx
+++ b/Project Spyn Gantt Chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tydng\Desktop\FSE-100-Team-4-Sheibanian\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D61AF071-C535-4150-9ED9-568683C9E2CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A30BFC49-D765-4C83-A223-307E081FCEA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project schedule" sheetId="11" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="61">
   <si>
     <t>Project SPYN</t>
   </si>
@@ -142,12 +142,6 @@
   </si>
   <si>
     <t>Milestone 2 - Sensor Calibration</t>
-  </si>
-  <si>
-    <t>Get Familiar with Sound Sensor</t>
-  </si>
-  <si>
-    <t>Get famliar with Color Sensor</t>
   </si>
   <si>
     <t>Figure Out How to Pick Up Guy</t>
@@ -1136,22 +1130,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="19" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="19" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="19" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1163,14 +1154,17 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="19" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="19" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="19" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -1862,8 +1856,8 @@
   </sheetPr>
   <dimension ref="A1:BL36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A5" zoomScale="81" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A12" zoomScale="81" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1889,29 +1883,28 @@
       <c r="E1" s="20"/>
       <c r="F1" s="21"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="115" t="s">
+      <c r="I1" s="114" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="116"/>
-      <c r="K1" s="116"/>
-      <c r="L1" s="116"/>
-      <c r="M1" s="116"/>
-      <c r="N1" s="116"/>
-      <c r="O1" s="116"/>
+      <c r="J1" s="115"/>
+      <c r="K1" s="115"/>
+      <c r="L1" s="115"/>
+      <c r="M1" s="115"/>
+      <c r="N1" s="115"/>
+      <c r="O1" s="115"/>
       <c r="P1" s="24"/>
-      <c r="Q1" s="114">
-        <f ca="1">TODAY()</f>
-        <v>45211</v>
-      </c>
-      <c r="R1" s="113"/>
-      <c r="S1" s="113"/>
-      <c r="T1" s="113"/>
-      <c r="U1" s="113"/>
-      <c r="V1" s="113"/>
-      <c r="W1" s="113"/>
-      <c r="X1" s="113"/>
-      <c r="Y1" s="113"/>
-      <c r="Z1" s="113"/>
+      <c r="Q1" s="113">
+        <v>45202</v>
+      </c>
+      <c r="R1" s="112"/>
+      <c r="S1" s="112"/>
+      <c r="T1" s="112"/>
+      <c r="U1" s="112"/>
+      <c r="V1" s="112"/>
+      <c r="W1" s="112"/>
+      <c r="X1" s="112"/>
+      <c r="Y1" s="112"/>
+      <c r="Z1" s="112"/>
     </row>
     <row r="2" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B2" s="96" t="s">
@@ -1923,28 +1916,28 @@
       <c r="D2" s="22"/>
       <c r="E2" s="23"/>
       <c r="F2" s="22"/>
-      <c r="I2" s="115" t="s">
+      <c r="I2" s="114" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="116"/>
-      <c r="K2" s="116"/>
-      <c r="L2" s="116"/>
-      <c r="M2" s="116"/>
-      <c r="N2" s="116"/>
-      <c r="O2" s="116"/>
+      <c r="J2" s="115"/>
+      <c r="K2" s="115"/>
+      <c r="L2" s="115"/>
+      <c r="M2" s="115"/>
+      <c r="N2" s="115"/>
+      <c r="O2" s="115"/>
       <c r="P2" s="24"/>
-      <c r="Q2" s="112">
+      <c r="Q2" s="111">
         <v>1</v>
       </c>
-      <c r="R2" s="113"/>
-      <c r="S2" s="113"/>
-      <c r="T2" s="113"/>
-      <c r="U2" s="113"/>
-      <c r="V2" s="113"/>
-      <c r="W2" s="113"/>
-      <c r="X2" s="113"/>
-      <c r="Y2" s="113"/>
-      <c r="Z2" s="113"/>
+      <c r="R2" s="112"/>
+      <c r="S2" s="112"/>
+      <c r="T2" s="112"/>
+      <c r="U2" s="112"/>
+      <c r="V2" s="112"/>
+      <c r="W2" s="112"/>
+      <c r="X2" s="112"/>
+      <c r="Y2" s="112"/>
+      <c r="Z2" s="112"/>
     </row>
     <row r="3" spans="1:64" s="26" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13"/>
@@ -1953,78 +1946,78 @@
       </c>
       <c r="D3" s="27"/>
       <c r="E3" s="28"/>
-      <c r="I3" s="117" t="s">
+      <c r="I3" s="106" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="118"/>
-      <c r="K3" s="118"/>
-      <c r="L3" s="118"/>
-      <c r="M3" s="118"/>
-      <c r="N3" s="118"/>
-      <c r="O3" s="118"/>
-      <c r="P3" s="117" t="s">
+      <c r="J3" s="107"/>
+      <c r="K3" s="107"/>
+      <c r="L3" s="107"/>
+      <c r="M3" s="107"/>
+      <c r="N3" s="107"/>
+      <c r="O3" s="107"/>
+      <c r="P3" s="106" t="s">
         <v>7</v>
       </c>
-      <c r="Q3" s="118"/>
-      <c r="R3" s="118"/>
-      <c r="S3" s="118"/>
-      <c r="T3" s="118"/>
-      <c r="U3" s="118"/>
-      <c r="V3" s="118"/>
-      <c r="W3" s="117" t="s">
+      <c r="Q3" s="107"/>
+      <c r="R3" s="107"/>
+      <c r="S3" s="107"/>
+      <c r="T3" s="107"/>
+      <c r="U3" s="107"/>
+      <c r="V3" s="107"/>
+      <c r="W3" s="106" t="s">
         <v>8</v>
       </c>
-      <c r="X3" s="118"/>
-      <c r="Y3" s="118"/>
-      <c r="Z3" s="118"/>
-      <c r="AA3" s="118"/>
-      <c r="AB3" s="118"/>
-      <c r="AC3" s="118"/>
-      <c r="AD3" s="117" t="s">
+      <c r="X3" s="107"/>
+      <c r="Y3" s="107"/>
+      <c r="Z3" s="107"/>
+      <c r="AA3" s="107"/>
+      <c r="AB3" s="107"/>
+      <c r="AC3" s="107"/>
+      <c r="AD3" s="106" t="s">
         <v>9</v>
       </c>
-      <c r="AE3" s="118"/>
-      <c r="AF3" s="118"/>
-      <c r="AG3" s="118"/>
-      <c r="AH3" s="118"/>
-      <c r="AI3" s="118"/>
-      <c r="AJ3" s="118"/>
-      <c r="AK3" s="117" t="s">
+      <c r="AE3" s="107"/>
+      <c r="AF3" s="107"/>
+      <c r="AG3" s="107"/>
+      <c r="AH3" s="107"/>
+      <c r="AI3" s="107"/>
+      <c r="AJ3" s="107"/>
+      <c r="AK3" s="106" t="s">
         <v>10</v>
       </c>
-      <c r="AL3" s="118"/>
-      <c r="AM3" s="118"/>
-      <c r="AN3" s="118"/>
-      <c r="AO3" s="118"/>
-      <c r="AP3" s="118"/>
-      <c r="AQ3" s="118"/>
-      <c r="AR3" s="117" t="s">
+      <c r="AL3" s="107"/>
+      <c r="AM3" s="107"/>
+      <c r="AN3" s="107"/>
+      <c r="AO3" s="107"/>
+      <c r="AP3" s="107"/>
+      <c r="AQ3" s="107"/>
+      <c r="AR3" s="106" t="s">
         <v>11</v>
       </c>
-      <c r="AS3" s="118"/>
-      <c r="AT3" s="118"/>
-      <c r="AU3" s="118"/>
-      <c r="AV3" s="118"/>
-      <c r="AW3" s="118"/>
-      <c r="AX3" s="118"/>
-      <c r="AY3" s="117" t="s">
+      <c r="AS3" s="107"/>
+      <c r="AT3" s="107"/>
+      <c r="AU3" s="107"/>
+      <c r="AV3" s="107"/>
+      <c r="AW3" s="107"/>
+      <c r="AX3" s="107"/>
+      <c r="AY3" s="106" t="s">
         <v>12</v>
       </c>
-      <c r="AZ3" s="118"/>
-      <c r="BA3" s="118"/>
-      <c r="BB3" s="118"/>
-      <c r="BC3" s="118"/>
-      <c r="BD3" s="118"/>
-      <c r="BE3" s="118"/>
-      <c r="BF3" s="117" t="s">
+      <c r="AZ3" s="107"/>
+      <c r="BA3" s="107"/>
+      <c r="BB3" s="107"/>
+      <c r="BC3" s="107"/>
+      <c r="BD3" s="107"/>
+      <c r="BE3" s="107"/>
+      <c r="BF3" s="106" t="s">
         <v>13</v>
       </c>
-      <c r="BG3" s="118"/>
-      <c r="BH3" s="118"/>
-      <c r="BI3" s="118"/>
-      <c r="BJ3" s="118"/>
-      <c r="BK3" s="118"/>
-      <c r="BL3" s="118"/>
+      <c r="BG3" s="107"/>
+      <c r="BH3" s="107"/>
+      <c r="BI3" s="107"/>
+      <c r="BJ3" s="107"/>
+      <c r="BK3" s="107"/>
+      <c r="BL3" s="107"/>
     </row>
     <row r="4" spans="1:64" s="26" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="14"/>
@@ -2032,558 +2025,558 @@
         <v>14</v>
       </c>
       <c r="E4" s="30"/>
-      <c r="I4" s="117">
-        <f ca="1">I5</f>
+      <c r="I4" s="106">
+        <f>I5</f>
+        <v>45201</v>
+      </c>
+      <c r="J4" s="107"/>
+      <c r="K4" s="107"/>
+      <c r="L4" s="107"/>
+      <c r="M4" s="107"/>
+      <c r="N4" s="107"/>
+      <c r="O4" s="107"/>
+      <c r="P4" s="107">
+        <f>P5</f>
         <v>45208</v>
       </c>
-      <c r="J4" s="118"/>
-      <c r="K4" s="118"/>
-      <c r="L4" s="118"/>
-      <c r="M4" s="118"/>
-      <c r="N4" s="118"/>
-      <c r="O4" s="118"/>
-      <c r="P4" s="118">
-        <f ca="1">P5</f>
+      <c r="Q4" s="107"/>
+      <c r="R4" s="107"/>
+      <c r="S4" s="107"/>
+      <c r="T4" s="107"/>
+      <c r="U4" s="107"/>
+      <c r="V4" s="107"/>
+      <c r="W4" s="107">
+        <f>W5</f>
         <v>45215</v>
       </c>
-      <c r="Q4" s="118"/>
-      <c r="R4" s="118"/>
-      <c r="S4" s="118"/>
-      <c r="T4" s="118"/>
-      <c r="U4" s="118"/>
-      <c r="V4" s="118"/>
-      <c r="W4" s="118">
-        <f ca="1">W5</f>
+      <c r="X4" s="107"/>
+      <c r="Y4" s="107"/>
+      <c r="Z4" s="107"/>
+      <c r="AA4" s="107"/>
+      <c r="AB4" s="107"/>
+      <c r="AC4" s="107"/>
+      <c r="AD4" s="107">
+        <f>AD5</f>
         <v>45222</v>
       </c>
-      <c r="X4" s="118"/>
-      <c r="Y4" s="118"/>
-      <c r="Z4" s="118"/>
-      <c r="AA4" s="118"/>
-      <c r="AB4" s="118"/>
-      <c r="AC4" s="118"/>
-      <c r="AD4" s="118">
-        <f ca="1">AD5</f>
+      <c r="AE4" s="107"/>
+      <c r="AF4" s="107"/>
+      <c r="AG4" s="107"/>
+      <c r="AH4" s="107"/>
+      <c r="AI4" s="107"/>
+      <c r="AJ4" s="107"/>
+      <c r="AK4" s="107">
+        <f>AK5</f>
         <v>45229</v>
       </c>
-      <c r="AE4" s="118"/>
-      <c r="AF4" s="118"/>
-      <c r="AG4" s="118"/>
-      <c r="AH4" s="118"/>
-      <c r="AI4" s="118"/>
-      <c r="AJ4" s="118"/>
-      <c r="AK4" s="118">
-        <f ca="1">AK5</f>
+      <c r="AL4" s="107"/>
+      <c r="AM4" s="107"/>
+      <c r="AN4" s="107"/>
+      <c r="AO4" s="107"/>
+      <c r="AP4" s="107"/>
+      <c r="AQ4" s="107"/>
+      <c r="AR4" s="107">
+        <f>AR5</f>
         <v>45236</v>
       </c>
-      <c r="AL4" s="118"/>
-      <c r="AM4" s="118"/>
-      <c r="AN4" s="118"/>
-      <c r="AO4" s="118"/>
-      <c r="AP4" s="118"/>
-      <c r="AQ4" s="118"/>
-      <c r="AR4" s="118">
-        <f ca="1">AR5</f>
+      <c r="AS4" s="107"/>
+      <c r="AT4" s="107"/>
+      <c r="AU4" s="107"/>
+      <c r="AV4" s="107"/>
+      <c r="AW4" s="107"/>
+      <c r="AX4" s="107"/>
+      <c r="AY4" s="107">
+        <f>AY5</f>
         <v>45243</v>
       </c>
-      <c r="AS4" s="118"/>
-      <c r="AT4" s="118"/>
-      <c r="AU4" s="118"/>
-      <c r="AV4" s="118"/>
-      <c r="AW4" s="118"/>
-      <c r="AX4" s="118"/>
-      <c r="AY4" s="118">
-        <f ca="1">AY5</f>
+      <c r="AZ4" s="107"/>
+      <c r="BA4" s="107"/>
+      <c r="BB4" s="107"/>
+      <c r="BC4" s="107"/>
+      <c r="BD4" s="107"/>
+      <c r="BE4" s="107"/>
+      <c r="BF4" s="107">
+        <f>BF5</f>
         <v>45250</v>
       </c>
-      <c r="AZ4" s="118"/>
-      <c r="BA4" s="118"/>
-      <c r="BB4" s="118"/>
-      <c r="BC4" s="118"/>
-      <c r="BD4" s="118"/>
-      <c r="BE4" s="118"/>
-      <c r="BF4" s="118">
-        <f ca="1">BF5</f>
-        <v>45257</v>
-      </c>
-      <c r="BG4" s="118"/>
-      <c r="BH4" s="118"/>
-      <c r="BI4" s="118"/>
-      <c r="BJ4" s="118"/>
-      <c r="BK4" s="118"/>
-      <c r="BL4" s="119"/>
+      <c r="BG4" s="107"/>
+      <c r="BH4" s="107"/>
+      <c r="BI4" s="107"/>
+      <c r="BJ4" s="107"/>
+      <c r="BK4" s="107"/>
+      <c r="BL4" s="108"/>
     </row>
     <row r="5" spans="1:64" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="106"/>
-      <c r="B5" s="107" t="s">
+      <c r="A5" s="116"/>
+      <c r="B5" s="117" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="109" t="s">
+      <c r="C5" s="119" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="111" t="s">
+      <c r="D5" s="109" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="111" t="s">
+      <c r="E5" s="109" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="111" t="s">
+      <c r="F5" s="109" t="s">
         <v>19</v>
       </c>
       <c r="I5" s="31">
-        <f ca="1">Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
+        <f>Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
+        <v>45201</v>
+      </c>
+      <c r="J5" s="31">
+        <f>I5+1</f>
+        <v>45202</v>
+      </c>
+      <c r="K5" s="31">
+        <f t="shared" ref="K5:AX5" si="0">J5+1</f>
+        <v>45203</v>
+      </c>
+      <c r="L5" s="31">
+        <f t="shared" si="0"/>
+        <v>45204</v>
+      </c>
+      <c r="M5" s="31">
+        <f t="shared" si="0"/>
+        <v>45205</v>
+      </c>
+      <c r="N5" s="31">
+        <f t="shared" si="0"/>
+        <v>45206</v>
+      </c>
+      <c r="O5" s="32">
+        <f t="shared" si="0"/>
+        <v>45207</v>
+      </c>
+      <c r="P5" s="33">
+        <f>O5+1</f>
         <v>45208</v>
       </c>
-      <c r="J5" s="31">
-        <f ca="1">I5+1</f>
+      <c r="Q5" s="31">
+        <f>P5+1</f>
         <v>45209</v>
       </c>
-      <c r="K5" s="31">
-        <f t="shared" ref="K5:AX5" ca="1" si="0">J5+1</f>
+      <c r="R5" s="31">
+        <f t="shared" si="0"/>
         <v>45210</v>
       </c>
-      <c r="L5" s="31">
-        <f t="shared" ca="1" si="0"/>
+      <c r="S5" s="31">
+        <f t="shared" si="0"/>
         <v>45211</v>
       </c>
-      <c r="M5" s="31">
-        <f t="shared" ca="1" si="0"/>
+      <c r="T5" s="31">
+        <f t="shared" si="0"/>
         <v>45212</v>
       </c>
-      <c r="N5" s="31">
-        <f t="shared" ca="1" si="0"/>
+      <c r="U5" s="31">
+        <f t="shared" si="0"/>
         <v>45213</v>
       </c>
-      <c r="O5" s="32">
-        <f t="shared" ca="1" si="0"/>
+      <c r="V5" s="32">
+        <f t="shared" si="0"/>
         <v>45214</v>
       </c>
-      <c r="P5" s="33">
-        <f ca="1">O5+1</f>
+      <c r="W5" s="33">
+        <f>V5+1</f>
         <v>45215</v>
       </c>
-      <c r="Q5" s="31">
-        <f ca="1">P5+1</f>
+      <c r="X5" s="31">
+        <f>W5+1</f>
         <v>45216</v>
       </c>
-      <c r="R5" s="31">
-        <f t="shared" ca="1" si="0"/>
+      <c r="Y5" s="31">
+        <f t="shared" si="0"/>
         <v>45217</v>
       </c>
-      <c r="S5" s="31">
-        <f t="shared" ca="1" si="0"/>
+      <c r="Z5" s="31">
+        <f t="shared" si="0"/>
         <v>45218</v>
       </c>
-      <c r="T5" s="31">
-        <f t="shared" ca="1" si="0"/>
+      <c r="AA5" s="31">
+        <f t="shared" si="0"/>
         <v>45219</v>
       </c>
-      <c r="U5" s="31">
-        <f t="shared" ca="1" si="0"/>
+      <c r="AB5" s="31">
+        <f t="shared" si="0"/>
         <v>45220</v>
       </c>
-      <c r="V5" s="32">
-        <f t="shared" ca="1" si="0"/>
+      <c r="AC5" s="32">
+        <f t="shared" si="0"/>
         <v>45221</v>
       </c>
-      <c r="W5" s="33">
-        <f ca="1">V5+1</f>
+      <c r="AD5" s="33">
+        <f>AC5+1</f>
         <v>45222</v>
       </c>
-      <c r="X5" s="31">
-        <f ca="1">W5+1</f>
+      <c r="AE5" s="31">
+        <f>AD5+1</f>
         <v>45223</v>
       </c>
-      <c r="Y5" s="31">
-        <f t="shared" ca="1" si="0"/>
+      <c r="AF5" s="31">
+        <f t="shared" si="0"/>
         <v>45224</v>
       </c>
-      <c r="Z5" s="31">
-        <f t="shared" ca="1" si="0"/>
+      <c r="AG5" s="31">
+        <f t="shared" si="0"/>
         <v>45225</v>
       </c>
-      <c r="AA5" s="31">
-        <f t="shared" ca="1" si="0"/>
+      <c r="AH5" s="31">
+        <f t="shared" si="0"/>
         <v>45226</v>
       </c>
-      <c r="AB5" s="31">
-        <f t="shared" ca="1" si="0"/>
+      <c r="AI5" s="31">
+        <f t="shared" si="0"/>
         <v>45227</v>
       </c>
-      <c r="AC5" s="32">
-        <f t="shared" ca="1" si="0"/>
+      <c r="AJ5" s="32">
+        <f t="shared" si="0"/>
         <v>45228</v>
       </c>
-      <c r="AD5" s="33">
-        <f ca="1">AC5+1</f>
+      <c r="AK5" s="33">
+        <f>AJ5+1</f>
         <v>45229</v>
       </c>
-      <c r="AE5" s="31">
-        <f ca="1">AD5+1</f>
+      <c r="AL5" s="31">
+        <f>AK5+1</f>
         <v>45230</v>
       </c>
-      <c r="AF5" s="31">
-        <f t="shared" ca="1" si="0"/>
+      <c r="AM5" s="31">
+        <f t="shared" si="0"/>
         <v>45231</v>
       </c>
-      <c r="AG5" s="31">
-        <f t="shared" ca="1" si="0"/>
+      <c r="AN5" s="31">
+        <f t="shared" si="0"/>
         <v>45232</v>
       </c>
-      <c r="AH5" s="31">
-        <f t="shared" ca="1" si="0"/>
+      <c r="AO5" s="31">
+        <f t="shared" si="0"/>
         <v>45233</v>
       </c>
-      <c r="AI5" s="31">
-        <f t="shared" ca="1" si="0"/>
+      <c r="AP5" s="31">
+        <f t="shared" si="0"/>
         <v>45234</v>
       </c>
-      <c r="AJ5" s="32">
-        <f t="shared" ca="1" si="0"/>
+      <c r="AQ5" s="32">
+        <f t="shared" si="0"/>
         <v>45235</v>
       </c>
-      <c r="AK5" s="33">
-        <f ca="1">AJ5+1</f>
+      <c r="AR5" s="33">
+        <f>AQ5+1</f>
         <v>45236</v>
       </c>
-      <c r="AL5" s="31">
-        <f ca="1">AK5+1</f>
+      <c r="AS5" s="31">
+        <f>AR5+1</f>
         <v>45237</v>
       </c>
-      <c r="AM5" s="31">
-        <f t="shared" ca="1" si="0"/>
+      <c r="AT5" s="31">
+        <f t="shared" si="0"/>
         <v>45238</v>
       </c>
-      <c r="AN5" s="31">
-        <f t="shared" ca="1" si="0"/>
+      <c r="AU5" s="31">
+        <f t="shared" si="0"/>
         <v>45239</v>
       </c>
-      <c r="AO5" s="31">
-        <f t="shared" ca="1" si="0"/>
+      <c r="AV5" s="31">
+        <f t="shared" si="0"/>
         <v>45240</v>
       </c>
-      <c r="AP5" s="31">
-        <f t="shared" ca="1" si="0"/>
+      <c r="AW5" s="31">
+        <f t="shared" si="0"/>
         <v>45241</v>
       </c>
-      <c r="AQ5" s="32">
-        <f t="shared" ca="1" si="0"/>
+      <c r="AX5" s="32">
+        <f t="shared" si="0"/>
         <v>45242</v>
       </c>
-      <c r="AR5" s="33">
-        <f ca="1">AQ5+1</f>
+      <c r="AY5" s="33">
+        <f>AX5+1</f>
         <v>45243</v>
       </c>
-      <c r="AS5" s="31">
-        <f ca="1">AR5+1</f>
+      <c r="AZ5" s="31">
+        <f>AY5+1</f>
         <v>45244</v>
       </c>
-      <c r="AT5" s="31">
-        <f t="shared" ca="1" si="0"/>
+      <c r="BA5" s="31">
+        <f t="shared" ref="BA5:BE5" si="1">AZ5+1</f>
         <v>45245</v>
       </c>
-      <c r="AU5" s="31">
-        <f t="shared" ca="1" si="0"/>
+      <c r="BB5" s="31">
+        <f t="shared" si="1"/>
         <v>45246</v>
       </c>
-      <c r="AV5" s="31">
-        <f t="shared" ca="1" si="0"/>
+      <c r="BC5" s="31">
+        <f t="shared" si="1"/>
         <v>45247</v>
       </c>
-      <c r="AW5" s="31">
-        <f t="shared" ca="1" si="0"/>
+      <c r="BD5" s="31">
+        <f t="shared" si="1"/>
         <v>45248</v>
       </c>
-      <c r="AX5" s="32">
-        <f t="shared" ca="1" si="0"/>
+      <c r="BE5" s="32">
+        <f t="shared" si="1"/>
         <v>45249</v>
       </c>
-      <c r="AY5" s="33">
-        <f ca="1">AX5+1</f>
+      <c r="BF5" s="33">
+        <f>BE5+1</f>
         <v>45250</v>
       </c>
-      <c r="AZ5" s="31">
-        <f ca="1">AY5+1</f>
+      <c r="BG5" s="31">
+        <f>BF5+1</f>
         <v>45251</v>
       </c>
-      <c r="BA5" s="31">
-        <f t="shared" ref="BA5:BE5" ca="1" si="1">AZ5+1</f>
+      <c r="BH5" s="31">
+        <f t="shared" ref="BH5:BL5" si="2">BG5+1</f>
         <v>45252</v>
       </c>
-      <c r="BB5" s="31">
-        <f t="shared" ca="1" si="1"/>
+      <c r="BI5" s="31">
+        <f t="shared" si="2"/>
         <v>45253</v>
       </c>
-      <c r="BC5" s="31">
-        <f t="shared" ca="1" si="1"/>
+      <c r="BJ5" s="31">
+        <f t="shared" si="2"/>
         <v>45254</v>
       </c>
-      <c r="BD5" s="31">
-        <f t="shared" ca="1" si="1"/>
+      <c r="BK5" s="31">
+        <f t="shared" si="2"/>
         <v>45255</v>
       </c>
-      <c r="BE5" s="32">
-        <f t="shared" ca="1" si="1"/>
+      <c r="BL5" s="31">
+        <f t="shared" si="2"/>
         <v>45256</v>
       </c>
-      <c r="BF5" s="33">
-        <f ca="1">BE5+1</f>
-        <v>45257</v>
-      </c>
-      <c r="BG5" s="31">
-        <f ca="1">BF5+1</f>
-        <v>45258</v>
-      </c>
-      <c r="BH5" s="31">
-        <f t="shared" ref="BH5:BL5" ca="1" si="2">BG5+1</f>
-        <v>45259</v>
-      </c>
-      <c r="BI5" s="31">
-        <f t="shared" ca="1" si="2"/>
-        <v>45260</v>
-      </c>
-      <c r="BJ5" s="31">
-        <f t="shared" ca="1" si="2"/>
-        <v>45261</v>
-      </c>
-      <c r="BK5" s="31">
-        <f t="shared" ca="1" si="2"/>
-        <v>45262</v>
-      </c>
-      <c r="BL5" s="31">
-        <f t="shared" ca="1" si="2"/>
-        <v>45263</v>
-      </c>
     </row>
     <row r="6" spans="1:64" s="26" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="106"/>
-      <c r="B6" s="108"/>
+      <c r="A6" s="116"/>
+      <c r="B6" s="118"/>
       <c r="C6" s="110"/>
       <c r="D6" s="110"/>
       <c r="E6" s="110"/>
       <c r="F6" s="110"/>
       <c r="I6" s="34" t="str">
-        <f t="shared" ref="I6:AN6" ca="1" si="3">LEFT(TEXT(I5,"ddd"),1)</f>
+        <f t="shared" ref="I6:AN6" si="3">LEFT(TEXT(I5,"ddd"),1)</f>
         <v>M</v>
       </c>
       <c r="J6" s="35" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>T</v>
       </c>
       <c r="K6" s="35" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>W</v>
       </c>
       <c r="L6" s="35" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>T</v>
       </c>
       <c r="M6" s="35" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>F</v>
       </c>
       <c r="N6" s="35" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>S</v>
       </c>
       <c r="O6" s="35" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>S</v>
       </c>
       <c r="P6" s="35" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>M</v>
       </c>
       <c r="Q6" s="35" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>T</v>
       </c>
       <c r="R6" s="35" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>W</v>
       </c>
       <c r="S6" s="35" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>T</v>
       </c>
       <c r="T6" s="35" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>F</v>
       </c>
       <c r="U6" s="35" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>S</v>
       </c>
       <c r="V6" s="35" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>S</v>
       </c>
       <c r="W6" s="35" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>M</v>
       </c>
       <c r="X6" s="35" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>T</v>
       </c>
       <c r="Y6" s="35" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>W</v>
       </c>
       <c r="Z6" s="35" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>T</v>
       </c>
       <c r="AA6" s="35" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>F</v>
       </c>
       <c r="AB6" s="35" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>S</v>
       </c>
       <c r="AC6" s="35" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>S</v>
       </c>
       <c r="AD6" s="35" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>M</v>
       </c>
       <c r="AE6" s="35" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>T</v>
       </c>
       <c r="AF6" s="35" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>W</v>
       </c>
       <c r="AG6" s="35" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>T</v>
       </c>
       <c r="AH6" s="35" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>F</v>
       </c>
       <c r="AI6" s="35" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>S</v>
       </c>
       <c r="AJ6" s="35" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>S</v>
       </c>
       <c r="AK6" s="35" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>M</v>
       </c>
       <c r="AL6" s="35" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>T</v>
       </c>
       <c r="AM6" s="35" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>W</v>
       </c>
       <c r="AN6" s="35" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>T</v>
       </c>
       <c r="AO6" s="35" t="str">
-        <f t="shared" ref="AO6:BL6" ca="1" si="4">LEFT(TEXT(AO5,"ddd"),1)</f>
+        <f t="shared" ref="AO6:BL6" si="4">LEFT(TEXT(AO5,"ddd"),1)</f>
         <v>F</v>
       </c>
       <c r="AP6" s="35" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="4"/>
         <v>S</v>
       </c>
       <c r="AQ6" s="35" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="4"/>
         <v>S</v>
       </c>
       <c r="AR6" s="35" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="4"/>
         <v>M</v>
       </c>
       <c r="AS6" s="35" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="4"/>
         <v>T</v>
       </c>
       <c r="AT6" s="35" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="4"/>
         <v>W</v>
       </c>
       <c r="AU6" s="35" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="4"/>
         <v>T</v>
       </c>
       <c r="AV6" s="35" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="4"/>
         <v>F</v>
       </c>
       <c r="AW6" s="35" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="4"/>
         <v>S</v>
       </c>
       <c r="AX6" s="35" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="4"/>
         <v>S</v>
       </c>
       <c r="AY6" s="35" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="4"/>
         <v>M</v>
       </c>
       <c r="AZ6" s="35" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="4"/>
         <v>T</v>
       </c>
       <c r="BA6" s="35" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="4"/>
         <v>W</v>
       </c>
       <c r="BB6" s="35" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="4"/>
         <v>T</v>
       </c>
       <c r="BC6" s="35" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="4"/>
         <v>F</v>
       </c>
       <c r="BD6" s="35" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="4"/>
         <v>S</v>
       </c>
       <c r="BE6" s="35" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="4"/>
         <v>S</v>
       </c>
       <c r="BF6" s="35" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="4"/>
         <v>M</v>
       </c>
       <c r="BG6" s="35" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="4"/>
         <v>T</v>
       </c>
       <c r="BH6" s="35" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="4"/>
         <v>W</v>
       </c>
       <c r="BI6" s="35" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="4"/>
         <v>T</v>
       </c>
       <c r="BJ6" s="35" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="4"/>
         <v>F</v>
       </c>
       <c r="BK6" s="35" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="4"/>
         <v>S</v>
       </c>
       <c r="BL6" s="36" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="4"/>
         <v>S</v>
       </c>
     </row>
@@ -2740,16 +2733,16 @@
         <v>1</v>
       </c>
       <c r="E9" s="50">
-        <f ca="1">Project_Start</f>
-        <v>45211</v>
+        <f>Project_Start</f>
+        <v>45202</v>
       </c>
       <c r="F9" s="50">
-        <f ca="1">E9+3</f>
-        <v>45214</v>
+        <f>E9+3</f>
+        <v>45205</v>
       </c>
       <c r="G9" s="17"/>
       <c r="H9" s="5">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="I9" s="51"/>
@@ -2821,16 +2814,16 @@
         <v>1</v>
       </c>
       <c r="E10" s="50">
-        <f ca="1">Project_Start</f>
-        <v>45211</v>
+        <f>Project_Start</f>
+        <v>45202</v>
       </c>
       <c r="F10" s="50">
-        <f ca="1">E10+3</f>
-        <v>45214</v>
+        <f>E10+3</f>
+        <v>45205</v>
       </c>
       <c r="G10" s="17"/>
       <c r="H10" s="5">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="I10" s="51"/>
@@ -2902,16 +2895,16 @@
         <v>1</v>
       </c>
       <c r="E11" s="55">
-        <f ca="1">F10</f>
-        <v>45214</v>
+        <f>F10</f>
+        <v>45205</v>
       </c>
       <c r="F11" s="55">
-        <f ca="1">E11+4</f>
-        <v>45218</v>
+        <f>E11+4</f>
+        <v>45209</v>
       </c>
       <c r="G11" s="17"/>
       <c r="H11" s="5">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="I11" s="51"/>
@@ -2983,16 +2976,16 @@
         <v>1</v>
       </c>
       <c r="E12" s="55">
-        <f ca="1">F11</f>
-        <v>45218</v>
+        <f>F11</f>
+        <v>45209</v>
       </c>
       <c r="F12" s="55">
-        <f ca="1">E12+2</f>
-        <v>45220</v>
+        <f>E12+2</f>
+        <v>45211</v>
       </c>
       <c r="G12" s="17"/>
       <c r="H12" s="5">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="I12" s="51"/>
@@ -3150,26 +3143,26 @@
     <row r="15" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14"/>
       <c r="B15" s="62" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C15" s="63" t="s">
         <v>26</v>
       </c>
       <c r="D15" s="64">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="E15" s="65">
         <f>E13+7</f>
         <v>45211</v>
       </c>
       <c r="F15" s="65">
-        <f>E15+3</f>
-        <v>45214</v>
+        <f>E15</f>
+        <v>45211</v>
       </c>
       <c r="G15" s="17"/>
       <c r="H15" s="5">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I15" s="51"/>
       <c r="J15" s="51"/>
@@ -3231,25 +3224,25 @@
     <row r="16" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="13"/>
       <c r="B16" s="62" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C16" s="63" t="s">
         <v>2</v>
       </c>
       <c r="D16" s="64">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="E16" s="65">
         <v>45211</v>
       </c>
       <c r="F16" s="65">
-        <f>E16-3</f>
-        <v>45208</v>
+        <f>E16+3</f>
+        <v>45214</v>
       </c>
       <c r="G16" s="17"/>
       <c r="H16" s="5">
         <f t="shared" si="5"/>
-        <v>-2</v>
+        <v>4</v>
       </c>
       <c r="I16" s="51"/>
       <c r="J16" s="51"/>
@@ -3311,13 +3304,13 @@
     <row r="17" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="13"/>
       <c r="B17" s="62" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C17" s="63" t="s">
         <v>24</v>
       </c>
       <c r="D17" s="64">
-        <v>0.5</v>
+        <v>0.85</v>
       </c>
       <c r="E17" s="65">
         <f>E15</f>
@@ -3392,26 +3385,26 @@
     <row r="18" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="13"/>
       <c r="B18" s="62" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C18" s="63" t="s">
         <v>28</v>
       </c>
       <c r="D18" s="64">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="E18" s="65">
         <f>E17</f>
         <v>45211</v>
       </c>
       <c r="F18" s="65">
-        <f>E18</f>
-        <v>45211</v>
+        <f>E18+2</f>
+        <v>45213</v>
       </c>
       <c r="G18" s="17"/>
       <c r="H18" s="5">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I18" s="51"/>
       <c r="J18" s="51"/>
@@ -3473,26 +3466,26 @@
     <row r="19" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="13"/>
       <c r="B19" s="62" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C19" s="63" t="s">
         <v>30</v>
       </c>
       <c r="D19" s="64">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="E19" s="65">
-        <f>E18</f>
-        <v>45211</v>
+        <f>E18-2</f>
+        <v>45209</v>
       </c>
       <c r="F19" s="65">
-        <f>E19+3</f>
-        <v>45214</v>
+        <f>E19</f>
+        <v>45209</v>
       </c>
       <c r="G19" s="17"/>
       <c r="H19" s="5">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I19" s="51"/>
       <c r="J19" s="51"/>
@@ -3554,7 +3547,7 @@
     <row r="20" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="13"/>
       <c r="B20" s="66" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C20" s="67"/>
       <c r="D20" s="68"/>
@@ -3625,23 +3618,23 @@
     <row r="21" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="13"/>
       <c r="B21" s="72" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C21" s="73" t="s">
         <v>24</v>
       </c>
       <c r="D21" s="74"/>
       <c r="E21" s="75">
-        <f ca="1">E9+15</f>
-        <v>45226</v>
+        <f>$E$9+15</f>
+        <v>45217</v>
       </c>
       <c r="F21" s="75">
-        <f ca="1">E21+5</f>
-        <v>45231</v>
+        <f>E21+5</f>
+        <v>45222</v>
       </c>
       <c r="G21" s="17"/>
       <c r="H21" s="5">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="I21" s="51"/>
@@ -3704,14 +3697,15 @@
     <row r="22" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="13"/>
       <c r="B22" s="72" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C22" s="73" t="s">
         <v>2</v>
       </c>
       <c r="D22" s="74"/>
       <c r="E22" s="75">
-        <v>45210</v>
+        <f t="shared" ref="E22:E25" si="6">$E$9+15</f>
+        <v>45217</v>
       </c>
       <c r="F22" s="75">
         <v>45215</v>
@@ -3719,7 +3713,7 @@
       <c r="G22" s="17"/>
       <c r="H22" s="5">
         <f t="shared" si="5"/>
-        <v>6</v>
+        <v>-1</v>
       </c>
       <c r="I22" s="51"/>
       <c r="J22" s="51"/>
@@ -3781,14 +3775,15 @@
     <row r="23" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="13"/>
       <c r="B23" s="72" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C23" s="73" t="s">
         <v>28</v>
       </c>
       <c r="D23" s="74"/>
       <c r="E23" s="75">
-        <v>45210</v>
+        <f t="shared" si="6"/>
+        <v>45217</v>
       </c>
       <c r="F23" s="75">
         <v>45215</v>
@@ -3796,7 +3791,7 @@
       <c r="G23" s="17"/>
       <c r="H23" s="5">
         <f t="shared" si="5"/>
-        <v>6</v>
+        <v>-1</v>
       </c>
       <c r="I23" s="51"/>
       <c r="J23" s="51"/>
@@ -3858,18 +3853,19 @@
     <row r="24" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="13"/>
       <c r="B24" s="72" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C24" s="73" t="s">
         <v>30</v>
       </c>
       <c r="D24" s="74"/>
       <c r="E24" s="75">
-        <v>45215</v>
+        <f t="shared" si="6"/>
+        <v>45217</v>
       </c>
       <c r="F24" s="75">
         <f>E24+4</f>
-        <v>45219</v>
+        <v>45221</v>
       </c>
       <c r="G24" s="17"/>
       <c r="H24" s="5">
@@ -3936,18 +3932,19 @@
     <row r="25" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="13"/>
       <c r="B25" s="72" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C25" s="73" t="s">
         <v>26</v>
       </c>
       <c r="D25" s="74"/>
       <c r="E25" s="75">
-        <v>45215</v>
+        <f t="shared" si="6"/>
+        <v>45217</v>
       </c>
       <c r="F25" s="75">
         <f>E25+4</f>
-        <v>45219</v>
+        <v>45221</v>
       </c>
       <c r="G25" s="17"/>
       <c r="H25" s="5">
@@ -4013,7 +4010,7 @@
     <row r="26" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="13"/>
       <c r="B26" s="76" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C26" s="77"/>
       <c r="D26" s="78"/>
@@ -4084,7 +4081,7 @@
     <row r="27" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="13"/>
       <c r="B27" s="82" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C27" s="83" t="s">
         <v>30</v>
@@ -4162,7 +4159,7 @@
     <row r="28" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="13"/>
       <c r="B28" s="82" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C28" s="83" t="s">
         <v>2</v>
@@ -4241,7 +4238,7 @@
     <row r="29" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="13"/>
       <c r="B29" s="82" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C29" s="83" t="s">
         <v>26</v>
@@ -4320,7 +4317,7 @@
     <row r="30" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="13"/>
       <c r="B30" s="82" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C30" s="83" t="s">
         <v>28</v>
@@ -4399,7 +4396,7 @@
     <row r="31" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="13"/>
       <c r="B31" s="82" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C31" s="83" t="s">
         <v>24</v>
@@ -4546,7 +4543,7 @@
     <row r="33" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="14"/>
       <c r="B33" s="90" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C33" s="91"/>
       <c r="D33" s="92"/>
@@ -4626,11 +4623,19 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="AD3:AJ3"/>
-    <mergeCell ref="AK3:AQ3"/>
-    <mergeCell ref="AR3:AX3"/>
-    <mergeCell ref="AY3:BE3"/>
-    <mergeCell ref="BF3:BL3"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="Q2:Z2"/>
+    <mergeCell ref="Q1:Z1"/>
+    <mergeCell ref="I1:O1"/>
+    <mergeCell ref="I2:O2"/>
+    <mergeCell ref="I3:O3"/>
+    <mergeCell ref="P3:V3"/>
+    <mergeCell ref="W3:AC3"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="I4:O4"/>
     <mergeCell ref="P4:V4"/>
@@ -4639,19 +4644,11 @@
     <mergeCell ref="AK4:AQ4"/>
     <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="AY4:BE4"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="Q2:Z2"/>
-    <mergeCell ref="Q1:Z1"/>
-    <mergeCell ref="I1:O1"/>
-    <mergeCell ref="I2:O2"/>
-    <mergeCell ref="I3:O3"/>
-    <mergeCell ref="P3:V3"/>
-    <mergeCell ref="W3:AC3"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="AD3:AJ3"/>
+    <mergeCell ref="AK3:AQ3"/>
+    <mergeCell ref="AR3:AX3"/>
+    <mergeCell ref="AY3:BE3"/>
+    <mergeCell ref="BF3:BL3"/>
   </mergeCells>
   <phoneticPr fontId="32" type="noConversion"/>
   <conditionalFormatting sqref="D7:D33">
@@ -4815,67 +4812,67 @@
     </row>
     <row r="4" spans="1:2" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.6">
       <c r="A4" s="101" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="74.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="102" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="101" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:2" s="7" customFormat="1" ht="205.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="103" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:2" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.6">
       <c r="A8" s="101" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="57" x14ac:dyDescent="0.2">
       <c r="A9" s="102" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:2" s="7" customFormat="1" ht="28.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="104" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:2" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.6">
       <c r="A11" s="101" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A12" s="102" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:2" s="7" customFormat="1" ht="28.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="104" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:2" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.6">
       <c r="A14" s="101" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="102" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A16" s="102" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
@@ -4921,6 +4918,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F010965E38DD9C4C9BE78EF37B7A5F63" ma:contentTypeVersion="3" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6e5a01bfcf6a1a5eee5a5ca1585b5a1a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="3e43f44c-3f4d-46ba-91a0-7c8ec4d7a2ca" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="00e6d9bda136d3704b372a6b2e4b23e5" ns3:_="">
     <xsd:import namespace="3e43f44c-3f4d-46ba-91a0-7c8ec4d7a2ca"/>
@@ -5058,15 +5064,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A82239A0-E68C-493F-BEE6-C77FEA397FD6}">
   <ds:schemaRefs>
@@ -5084,6 +5081,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A800D70D-3EC9-4DB9-B9D8-9E383CE8B438}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5101,14 +5106,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata"/>
 </file>
</xml_diff>

<commit_message>
Updated control.m and the Gantt chart
The code should be mostly autonomous, just need to adjust some variables such as distance from wall and such.
</commit_message>
<xml_diff>
--- a/Project Spyn Gantt Chart.xlsx
+++ b/Project Spyn Gantt Chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tydng\Desktop\FSE-100-Team-4-Sheibanian\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7751C0F5-A460-4372-9D13-118D5DCB9080}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3832A88B-1E0B-4526-9EDC-7ED7FA365562}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project schedule" sheetId="11" r:id="rId1"/>
@@ -245,7 +245,7 @@
     <t>Full Autonomous Run</t>
   </si>
   <si>
-    <t>Work onweight distribution of Car</t>
+    <t>Work on weight distribution of Car</t>
   </si>
 </sst>
 </file>
@@ -1120,22 +1120,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="3" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="17" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1147,14 +1144,17 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="17" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="17" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="17" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -1954,8 +1954,8 @@
   </sheetPr>
   <dimension ref="A1:BL36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A17" zoomScale="81" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A9" zoomScale="81" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1981,28 +1981,28 @@
       <c r="E1" s="16"/>
       <c r="F1" s="17"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="111" t="s">
+      <c r="I1" s="110" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="112"/>
-      <c r="K1" s="112"/>
-      <c r="L1" s="112"/>
-      <c r="M1" s="112"/>
-      <c r="N1" s="112"/>
-      <c r="O1" s="112"/>
+      <c r="J1" s="111"/>
+      <c r="K1" s="111"/>
+      <c r="L1" s="111"/>
+      <c r="M1" s="111"/>
+      <c r="N1" s="111"/>
+      <c r="O1" s="111"/>
       <c r="P1" s="20"/>
-      <c r="Q1" s="110">
+      <c r="Q1" s="109">
         <v>45202</v>
       </c>
-      <c r="R1" s="109"/>
-      <c r="S1" s="109"/>
-      <c r="T1" s="109"/>
-      <c r="U1" s="109"/>
-      <c r="V1" s="109"/>
-      <c r="W1" s="109"/>
-      <c r="X1" s="109"/>
-      <c r="Y1" s="109"/>
-      <c r="Z1" s="109"/>
+      <c r="R1" s="108"/>
+      <c r="S1" s="108"/>
+      <c r="T1" s="108"/>
+      <c r="U1" s="108"/>
+      <c r="V1" s="108"/>
+      <c r="W1" s="108"/>
+      <c r="X1" s="108"/>
+      <c r="Y1" s="108"/>
+      <c r="Z1" s="108"/>
     </row>
     <row r="2" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B2" s="92" t="s">
@@ -2014,28 +2014,28 @@
       <c r="D2" s="18"/>
       <c r="E2" s="19"/>
       <c r="F2" s="18"/>
-      <c r="I2" s="111" t="s">
+      <c r="I2" s="110" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="112"/>
-      <c r="K2" s="112"/>
-      <c r="L2" s="112"/>
-      <c r="M2" s="112"/>
-      <c r="N2" s="112"/>
-      <c r="O2" s="112"/>
+      <c r="J2" s="111"/>
+      <c r="K2" s="111"/>
+      <c r="L2" s="111"/>
+      <c r="M2" s="111"/>
+      <c r="N2" s="111"/>
+      <c r="O2" s="111"/>
       <c r="P2" s="20"/>
-      <c r="Q2" s="108">
+      <c r="Q2" s="107">
         <v>1</v>
       </c>
-      <c r="R2" s="109"/>
-      <c r="S2" s="109"/>
-      <c r="T2" s="109"/>
-      <c r="U2" s="109"/>
-      <c r="V2" s="109"/>
-      <c r="W2" s="109"/>
-      <c r="X2" s="109"/>
-      <c r="Y2" s="109"/>
-      <c r="Z2" s="109"/>
+      <c r="R2" s="108"/>
+      <c r="S2" s="108"/>
+      <c r="T2" s="108"/>
+      <c r="U2" s="108"/>
+      <c r="V2" s="108"/>
+      <c r="W2" s="108"/>
+      <c r="X2" s="108"/>
+      <c r="Y2" s="108"/>
+      <c r="Z2" s="108"/>
     </row>
     <row r="3" spans="1:64" s="22" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
@@ -2044,78 +2044,78 @@
       </c>
       <c r="D3" s="23"/>
       <c r="E3" s="24"/>
-      <c r="I3" s="113" t="s">
+      <c r="I3" s="102" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="114"/>
-      <c r="K3" s="114"/>
-      <c r="L3" s="114"/>
-      <c r="M3" s="114"/>
-      <c r="N3" s="114"/>
-      <c r="O3" s="114"/>
-      <c r="P3" s="113" t="s">
+      <c r="J3" s="103"/>
+      <c r="K3" s="103"/>
+      <c r="L3" s="103"/>
+      <c r="M3" s="103"/>
+      <c r="N3" s="103"/>
+      <c r="O3" s="103"/>
+      <c r="P3" s="102" t="s">
         <v>7</v>
       </c>
-      <c r="Q3" s="114"/>
-      <c r="R3" s="114"/>
-      <c r="S3" s="114"/>
-      <c r="T3" s="114"/>
-      <c r="U3" s="114"/>
-      <c r="V3" s="114"/>
-      <c r="W3" s="113" t="s">
+      <c r="Q3" s="103"/>
+      <c r="R3" s="103"/>
+      <c r="S3" s="103"/>
+      <c r="T3" s="103"/>
+      <c r="U3" s="103"/>
+      <c r="V3" s="103"/>
+      <c r="W3" s="102" t="s">
         <v>8</v>
       </c>
-      <c r="X3" s="114"/>
-      <c r="Y3" s="114"/>
-      <c r="Z3" s="114"/>
-      <c r="AA3" s="114"/>
-      <c r="AB3" s="114"/>
-      <c r="AC3" s="114"/>
-      <c r="AD3" s="113" t="s">
+      <c r="X3" s="103"/>
+      <c r="Y3" s="103"/>
+      <c r="Z3" s="103"/>
+      <c r="AA3" s="103"/>
+      <c r="AB3" s="103"/>
+      <c r="AC3" s="103"/>
+      <c r="AD3" s="102" t="s">
         <v>9</v>
       </c>
-      <c r="AE3" s="114"/>
-      <c r="AF3" s="114"/>
-      <c r="AG3" s="114"/>
-      <c r="AH3" s="114"/>
-      <c r="AI3" s="114"/>
-      <c r="AJ3" s="114"/>
-      <c r="AK3" s="113" t="s">
+      <c r="AE3" s="103"/>
+      <c r="AF3" s="103"/>
+      <c r="AG3" s="103"/>
+      <c r="AH3" s="103"/>
+      <c r="AI3" s="103"/>
+      <c r="AJ3" s="103"/>
+      <c r="AK3" s="102" t="s">
         <v>10</v>
       </c>
-      <c r="AL3" s="114"/>
-      <c r="AM3" s="114"/>
-      <c r="AN3" s="114"/>
-      <c r="AO3" s="114"/>
-      <c r="AP3" s="114"/>
-      <c r="AQ3" s="114"/>
-      <c r="AR3" s="113" t="s">
+      <c r="AL3" s="103"/>
+      <c r="AM3" s="103"/>
+      <c r="AN3" s="103"/>
+      <c r="AO3" s="103"/>
+      <c r="AP3" s="103"/>
+      <c r="AQ3" s="103"/>
+      <c r="AR3" s="102" t="s">
         <v>11</v>
       </c>
-      <c r="AS3" s="114"/>
-      <c r="AT3" s="114"/>
-      <c r="AU3" s="114"/>
-      <c r="AV3" s="114"/>
-      <c r="AW3" s="114"/>
-      <c r="AX3" s="114"/>
-      <c r="AY3" s="113" t="s">
+      <c r="AS3" s="103"/>
+      <c r="AT3" s="103"/>
+      <c r="AU3" s="103"/>
+      <c r="AV3" s="103"/>
+      <c r="AW3" s="103"/>
+      <c r="AX3" s="103"/>
+      <c r="AY3" s="102" t="s">
         <v>12</v>
       </c>
-      <c r="AZ3" s="114"/>
-      <c r="BA3" s="114"/>
-      <c r="BB3" s="114"/>
-      <c r="BC3" s="114"/>
-      <c r="BD3" s="114"/>
-      <c r="BE3" s="114"/>
-      <c r="BF3" s="113" t="s">
+      <c r="AZ3" s="103"/>
+      <c r="BA3" s="103"/>
+      <c r="BB3" s="103"/>
+      <c r="BC3" s="103"/>
+      <c r="BD3" s="103"/>
+      <c r="BE3" s="103"/>
+      <c r="BF3" s="102" t="s">
         <v>13</v>
       </c>
-      <c r="BG3" s="114"/>
-      <c r="BH3" s="114"/>
-      <c r="BI3" s="114"/>
-      <c r="BJ3" s="114"/>
-      <c r="BK3" s="114"/>
-      <c r="BL3" s="114"/>
+      <c r="BG3" s="103"/>
+      <c r="BH3" s="103"/>
+      <c r="BI3" s="103"/>
+      <c r="BJ3" s="103"/>
+      <c r="BK3" s="103"/>
+      <c r="BL3" s="103"/>
     </row>
     <row r="4" spans="1:64" s="22" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="12"/>
@@ -2123,102 +2123,102 @@
         <v>14</v>
       </c>
       <c r="E4" s="26"/>
-      <c r="I4" s="113">
+      <c r="I4" s="102">
         <f>I5</f>
         <v>45201</v>
       </c>
-      <c r="J4" s="114"/>
-      <c r="K4" s="114"/>
-      <c r="L4" s="114"/>
-      <c r="M4" s="114"/>
-      <c r="N4" s="114"/>
-      <c r="O4" s="114"/>
-      <c r="P4" s="114">
+      <c r="J4" s="103"/>
+      <c r="K4" s="103"/>
+      <c r="L4" s="103"/>
+      <c r="M4" s="103"/>
+      <c r="N4" s="103"/>
+      <c r="O4" s="103"/>
+      <c r="P4" s="103">
         <f>P5</f>
         <v>45208</v>
       </c>
-      <c r="Q4" s="114"/>
-      <c r="R4" s="114"/>
-      <c r="S4" s="114"/>
-      <c r="T4" s="114"/>
-      <c r="U4" s="114"/>
-      <c r="V4" s="114"/>
-      <c r="W4" s="114">
+      <c r="Q4" s="103"/>
+      <c r="R4" s="103"/>
+      <c r="S4" s="103"/>
+      <c r="T4" s="103"/>
+      <c r="U4" s="103"/>
+      <c r="V4" s="103"/>
+      <c r="W4" s="103">
         <f>W5</f>
         <v>45215</v>
       </c>
-      <c r="X4" s="114"/>
-      <c r="Y4" s="114"/>
-      <c r="Z4" s="114"/>
-      <c r="AA4" s="114"/>
-      <c r="AB4" s="114"/>
-      <c r="AC4" s="114"/>
-      <c r="AD4" s="114">
+      <c r="X4" s="103"/>
+      <c r="Y4" s="103"/>
+      <c r="Z4" s="103"/>
+      <c r="AA4" s="103"/>
+      <c r="AB4" s="103"/>
+      <c r="AC4" s="103"/>
+      <c r="AD4" s="103">
         <f>AD5</f>
         <v>45222</v>
       </c>
-      <c r="AE4" s="114"/>
-      <c r="AF4" s="114"/>
-      <c r="AG4" s="114"/>
-      <c r="AH4" s="114"/>
-      <c r="AI4" s="114"/>
-      <c r="AJ4" s="114"/>
-      <c r="AK4" s="114">
+      <c r="AE4" s="103"/>
+      <c r="AF4" s="103"/>
+      <c r="AG4" s="103"/>
+      <c r="AH4" s="103"/>
+      <c r="AI4" s="103"/>
+      <c r="AJ4" s="103"/>
+      <c r="AK4" s="103">
         <f>AK5</f>
         <v>45229</v>
       </c>
-      <c r="AL4" s="114"/>
-      <c r="AM4" s="114"/>
-      <c r="AN4" s="114"/>
-      <c r="AO4" s="114"/>
-      <c r="AP4" s="114"/>
-      <c r="AQ4" s="114"/>
-      <c r="AR4" s="114">
+      <c r="AL4" s="103"/>
+      <c r="AM4" s="103"/>
+      <c r="AN4" s="103"/>
+      <c r="AO4" s="103"/>
+      <c r="AP4" s="103"/>
+      <c r="AQ4" s="103"/>
+      <c r="AR4" s="103">
         <f>AR5</f>
         <v>45236</v>
       </c>
-      <c r="AS4" s="114"/>
-      <c r="AT4" s="114"/>
-      <c r="AU4" s="114"/>
-      <c r="AV4" s="114"/>
-      <c r="AW4" s="114"/>
-      <c r="AX4" s="114"/>
-      <c r="AY4" s="114">
+      <c r="AS4" s="103"/>
+      <c r="AT4" s="103"/>
+      <c r="AU4" s="103"/>
+      <c r="AV4" s="103"/>
+      <c r="AW4" s="103"/>
+      <c r="AX4" s="103"/>
+      <c r="AY4" s="103">
         <f>AY5</f>
         <v>45243</v>
       </c>
-      <c r="AZ4" s="114"/>
-      <c r="BA4" s="114"/>
-      <c r="BB4" s="114"/>
-      <c r="BC4" s="114"/>
-      <c r="BD4" s="114"/>
-      <c r="BE4" s="114"/>
-      <c r="BF4" s="114">
+      <c r="AZ4" s="103"/>
+      <c r="BA4" s="103"/>
+      <c r="BB4" s="103"/>
+      <c r="BC4" s="103"/>
+      <c r="BD4" s="103"/>
+      <c r="BE4" s="103"/>
+      <c r="BF4" s="103">
         <f>BF5</f>
         <v>45250</v>
       </c>
-      <c r="BG4" s="114"/>
-      <c r="BH4" s="114"/>
-      <c r="BI4" s="114"/>
-      <c r="BJ4" s="114"/>
-      <c r="BK4" s="114"/>
-      <c r="BL4" s="115"/>
+      <c r="BG4" s="103"/>
+      <c r="BH4" s="103"/>
+      <c r="BI4" s="103"/>
+      <c r="BJ4" s="103"/>
+      <c r="BK4" s="103"/>
+      <c r="BL4" s="104"/>
     </row>
     <row r="5" spans="1:64" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="102"/>
-      <c r="B5" s="103" t="s">
+      <c r="A5" s="112"/>
+      <c r="B5" s="113" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="105" t="s">
+      <c r="C5" s="115" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="107" t="s">
+      <c r="D5" s="105" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="107" t="s">
+      <c r="E5" s="105" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="107" t="s">
+      <c r="F5" s="105" t="s">
         <v>19</v>
       </c>
       <c r="I5" s="27">
@@ -2447,8 +2447,8 @@
       </c>
     </row>
     <row r="6" spans="1:64" s="22" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="102"/>
-      <c r="B6" s="104"/>
+      <c r="A6" s="112"/>
+      <c r="B6" s="114"/>
       <c r="C6" s="106"/>
       <c r="D6" s="106"/>
       <c r="E6" s="106"/>
@@ -3813,7 +3813,7 @@
         <v>30</v>
       </c>
       <c r="D22" s="60">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="E22" s="61">
         <f>E19-2</f>
@@ -4126,19 +4126,19 @@
         <v>28</v>
       </c>
       <c r="D26" s="70">
-        <v>0.65</v>
+        <v>0.8</v>
       </c>
       <c r="E26" s="71">
         <f t="shared" si="6"/>
         <v>45217</v>
       </c>
       <c r="F26" s="71">
-        <v>45237</v>
+        <v>45243</v>
       </c>
       <c r="G26" s="13"/>
       <c r="H26" s="3">
         <f t="shared" si="5"/>
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="I26" s="47"/>
       <c r="J26" s="47"/>
@@ -4972,11 +4972,19 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="AD3:AJ3"/>
-    <mergeCell ref="AK3:AQ3"/>
-    <mergeCell ref="AR3:AX3"/>
-    <mergeCell ref="AY3:BE3"/>
-    <mergeCell ref="BF3:BL3"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="Q2:Z2"/>
+    <mergeCell ref="Q1:Z1"/>
+    <mergeCell ref="I1:O1"/>
+    <mergeCell ref="I2:O2"/>
+    <mergeCell ref="I3:O3"/>
+    <mergeCell ref="P3:V3"/>
+    <mergeCell ref="W3:AC3"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="I4:O4"/>
     <mergeCell ref="P4:V4"/>
@@ -4985,19 +4993,11 @@
     <mergeCell ref="AK4:AQ4"/>
     <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="AY4:BE4"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="Q2:Z2"/>
-    <mergeCell ref="Q1:Z1"/>
-    <mergeCell ref="I1:O1"/>
-    <mergeCell ref="I2:O2"/>
-    <mergeCell ref="I3:O3"/>
-    <mergeCell ref="P3:V3"/>
-    <mergeCell ref="W3:AC3"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="AD3:AJ3"/>
+    <mergeCell ref="AK3:AQ3"/>
+    <mergeCell ref="AR3:AX3"/>
+    <mergeCell ref="AY3:BE3"/>
+    <mergeCell ref="BF3:BL3"/>
   </mergeCells>
   <phoneticPr fontId="30" type="noConversion"/>
   <conditionalFormatting sqref="D7:D36">
@@ -5303,6 +5303,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F010965E38DD9C4C9BE78EF37B7A5F63" ma:contentTypeVersion="3" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6e5a01bfcf6a1a5eee5a5ca1585b5a1a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="3e43f44c-3f4d-46ba-91a0-7c8ec4d7a2ca" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="00e6d9bda136d3704b372a6b2e4b23e5" ns3:_="">
     <xsd:import namespace="3e43f44c-3f4d-46ba-91a0-7c8ec4d7a2ca"/>
@@ -5440,15 +5449,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A82239A0-E68C-493F-BEE6-C77FEA397FD6}">
   <ds:schemaRefs>
@@ -5466,6 +5466,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A800D70D-3EC9-4DB9-B9D8-9E383CE8B438}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5483,14 +5491,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata"/>
 </file>
</xml_diff>